<commit_message>
'Balance' and 'PSCAD compilers' tabs removed
</commit_message>
<xml_diff>
--- a/PSCAD/DK1_DSO_D/TestCases.xlsx
+++ b/PSCAD/DK1_DSO_D/TestCases.xlsx
@@ -5,17 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MKT.ENERGINET\Desktop\PP-MTB-Alpha\PP-MTB PSCAD\DK1_DSO_D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\energinet.local\endk_funktion\Projekter\EffektGruppen\13_Medarbejdermapper\CVL\PP-MTB\PSCAD\DK1_DSO_D\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="350"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="2" r:id="rId1"/>
     <sheet name="Cases" sheetId="1" r:id="rId2"/>
-    <sheet name="Balance" sheetId="3" r:id="rId3"/>
-    <sheet name="PSCAD Compliers" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Input!$A$1:$M$2</definedName>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="125">
   <si>
     <t>PrefCtrl</t>
   </si>
@@ -171,9 +169,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>Balance</t>
-  </si>
-  <si>
     <t>P0</t>
   </si>
   <si>
@@ -264,25 +259,12 @@
     <t>Qmode_PF: Power factor control</t>
   </si>
   <si>
-    <t>Additional information:
-An overview of all the balances tested</t>
-  </si>
-  <si>
     <t>Qmode</t>
   </si>
   <si>
     <t>InitValue</t>
   </si>
   <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>PF</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
     <t>TestType</t>
   </si>
   <si>
@@ -415,139 +397,10 @@
     <t>TotalCases</t>
   </si>
   <si>
-    <t>Intel(R) Visual Fortran Compiler XE 12.1.7.371</t>
-  </si>
-  <si>
-    <t>GFortran 4.6.2</t>
-  </si>
-  <si>
-    <t>GFortran 8.1</t>
-  </si>
-  <si>
-    <t>GFortran 8.1 (64-bit)</t>
-  </si>
-  <si>
     <t>Intel(R) Visual Fortran Compiler XE 15.0.1.148</t>
   </si>
   <si>
-    <t>Intel(R) Visual Fortran Compiler XE 15.0.1.148 (64-bit)</t>
-  </si>
-  <si>
-    <t>Intel(R) Visual Fortran Compiler XE 15.0.5.280</t>
-  </si>
-  <si>
-    <t>Intel(R) Visual Fortran Compiler XE 15.0.5.280 (64-bit)</t>
-  </si>
-  <si>
     <t>Note:</t>
-  </si>
-  <si>
-    <t>Servers:</t>
-  </si>
-  <si>
-    <t>X0133P01</t>
-  </si>
-  <si>
-    <t>Y0133P03</t>
-  </si>
-  <si>
-    <t>Y0133P01</t>
-  </si>
-  <si>
-    <t>Y0133P02</t>
-  </si>
-  <si>
-    <t>Compliers:</t>
-  </si>
-  <si>
-    <t>The compliers are different on different servers at Energinet.</t>
-  </si>
-  <si>
-    <r>
-      <t>Intel(R) Visual Fortran Compiler XE 15.0.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>5.280</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Intel(R) Visual Fortran Compiler XE 15.0.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>5.280</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (64-bit)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Intel(R) Visual Fortran Compiler XE 15.0.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.148</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Intel(R) Visual Fortran Compiler XE 15.0.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.148</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (64-bit)</t>
-    </r>
-  </si>
-  <si>
-    <t>See 'PSCAD Compliers' sheet for guidance</t>
   </si>
   <si>
     <t>Volley</t>
@@ -569,7 +422,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,13 +432,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -608,14 +454,6 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -683,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -706,22 +544,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -730,16 +556,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -757,7 +577,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -769,13 +589,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -792,17 +612,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1261,18 +1071,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="15" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="8" style="15" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="15"/>
+    <col min="2" max="2" width="6.42578125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="8" style="11" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="11"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
@@ -1282,64 +1090,64 @@
     <col min="13" max="13" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="14" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="C1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="D1" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="E1" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="K1" s="19" t="s">
+      <c r="J1" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="N1" s="13" t="s">
         <v>121</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="15">
+      <c r="B2" s="11">
         <v>10</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="11">
         <v>10</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="11">
         <v>62.5</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="11">
         <v>5</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="11">
         <v>15</v>
       </c>
       <c r="G2">
@@ -1352,10 +1160,10 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="K2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="L2">
         <v>2</v>
@@ -1368,36 +1176,33 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G4" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="K4" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="N4" s="32" t="s">
-        <v>146</v>
+      <c r="G4" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
+      <c r="G5" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G6" s="32" t="s">
-        <v>71</v>
+      <c r="G6" s="26" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G7" s="32" t="s">
-        <v>72</v>
+      <c r="G7" s="26" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G8" s="32" t="s">
-        <v>73</v>
+      <c r="G8" s="26" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1411,7 +1216,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'PSCAD Compliers'!$A$1:$A$8</xm:f>
+            <xm:f>#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>K2</xm:sqref>
         </x14:dataValidation>
@@ -1468,67 +1273,67 @@
         <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="23" t="s">
+      <c r="D1" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q1" s="24" t="s">
+      <c r="P1" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q1" s="18" t="s">
         <v>8</v>
       </c>
       <c r="R1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="8" t="s">
         <v>15</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>16</v>
@@ -1537,7 +1342,7 @@
         <v>17</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Z1" s="4" t="s">
         <v>18</v>
@@ -1546,7 +1351,7 @@
         <v>19</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>20</v>
@@ -1555,7 +1360,7 @@
         <v>21</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>22</v>
@@ -1564,72 +1369,72 @@
         <v>30</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>31</v>
       </c>
       <c r="AJ1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="23">
-        <v>1</v>
-      </c>
-      <c r="D2" s="23">
-        <v>1</v>
-      </c>
-      <c r="E2" s="25">
-        <v>1</v>
-      </c>
-      <c r="F2" s="26">
+        <v>76</v>
+      </c>
+      <c r="C2" s="17">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17">
+        <v>1</v>
+      </c>
+      <c r="E2" s="19">
+        <v>1</v>
+      </c>
+      <c r="F2" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G2" s="25">
-        <v>0</v>
-      </c>
-      <c r="H2" s="23">
-        <v>0</v>
-      </c>
-      <c r="I2" s="23">
-        <v>0</v>
-      </c>
-      <c r="J2" s="23">
+      <c r="G2" s="19">
+        <v>0</v>
+      </c>
+      <c r="H2" s="17">
+        <v>0</v>
+      </c>
+      <c r="I2" s="17">
+        <v>0</v>
+      </c>
+      <c r="J2" s="17">
         <v>7</v>
       </c>
       <c r="K2" s="7">
         <v>0.01</v>
       </c>
-      <c r="L2" s="27">
+      <c r="L2" s="21">
         <v>0.15</v>
       </c>
-      <c r="M2" s="23">
-        <v>0</v>
-      </c>
-      <c r="N2" s="23">
-        <v>0</v>
-      </c>
-      <c r="O2" s="23">
-        <v>0</v>
-      </c>
-      <c r="P2" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="23">
+      <c r="M2" s="17">
+        <v>0</v>
+      </c>
+      <c r="N2" s="17">
+        <v>0</v>
+      </c>
+      <c r="O2" s="17">
+        <v>0</v>
+      </c>
+      <c r="P2" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="17">
         <v>4</v>
       </c>
       <c r="R2" s="4">
@@ -1641,7 +1446,7 @@
       <c r="T2" s="4">
         <v>0</v>
       </c>
-      <c r="U2" s="21">
+      <c r="U2" s="15">
         <v>4</v>
       </c>
       <c r="V2" s="3">
@@ -1698,55 +1503,55 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="23">
+        <v>77</v>
+      </c>
+      <c r="C3" s="17">
         <v>2</v>
       </c>
-      <c r="D3" s="23">
-        <v>1</v>
-      </c>
-      <c r="E3" s="25">
-        <v>1</v>
-      </c>
-      <c r="F3" s="26">
+      <c r="D3" s="17">
+        <v>1</v>
+      </c>
+      <c r="E3" s="19">
+        <v>1</v>
+      </c>
+      <c r="F3" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G3" s="25">
-        <v>0</v>
-      </c>
-      <c r="H3" s="23">
-        <v>0</v>
-      </c>
-      <c r="I3" s="23">
-        <v>0</v>
-      </c>
-      <c r="J3" s="23">
+      <c r="G3" s="19">
+        <v>0</v>
+      </c>
+      <c r="H3" s="17">
+        <v>0</v>
+      </c>
+      <c r="I3" s="17">
+        <v>0</v>
+      </c>
+      <c r="J3" s="17">
         <v>7</v>
       </c>
-      <c r="K3" s="27">
+      <c r="K3" s="21">
         <v>0.2</v>
       </c>
-      <c r="L3" s="27">
+      <c r="L3" s="21">
         <v>0.45</v>
       </c>
-      <c r="M3" s="23">
-        <v>0</v>
-      </c>
-      <c r="N3" s="23">
-        <v>0</v>
-      </c>
-      <c r="O3" s="23">
-        <v>0</v>
-      </c>
-      <c r="P3" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="23">
+      <c r="M3" s="17">
+        <v>0</v>
+      </c>
+      <c r="N3" s="17">
+        <v>0</v>
+      </c>
+      <c r="O3" s="17">
+        <v>0</v>
+      </c>
+      <c r="P3" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="17">
         <v>4</v>
       </c>
       <c r="R3" s="4">
@@ -1758,7 +1563,7 @@
       <c r="T3" s="4">
         <v>0</v>
       </c>
-      <c r="U3" s="21">
+      <c r="U3" s="15">
         <v>4</v>
       </c>
       <c r="V3" s="3">
@@ -1815,55 +1620,55 @@
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="23">
+        <v>78</v>
+      </c>
+      <c r="C4" s="17">
         <v>3</v>
       </c>
-      <c r="D4" s="23">
-        <v>1</v>
-      </c>
-      <c r="E4" s="25">
-        <v>1</v>
-      </c>
-      <c r="F4" s="26">
+      <c r="D4" s="17">
+        <v>1</v>
+      </c>
+      <c r="E4" s="19">
+        <v>1</v>
+      </c>
+      <c r="F4" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G4" s="25">
-        <v>0</v>
-      </c>
-      <c r="H4" s="23">
-        <v>0</v>
-      </c>
-      <c r="I4" s="23">
-        <v>0</v>
-      </c>
-      <c r="J4" s="23">
+      <c r="G4" s="19">
+        <v>0</v>
+      </c>
+      <c r="H4" s="17">
+        <v>0</v>
+      </c>
+      <c r="I4" s="17">
+        <v>0</v>
+      </c>
+      <c r="J4" s="17">
         <v>4</v>
       </c>
-      <c r="K4" s="28">
+      <c r="K4" s="22">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="L4" s="27">
+      <c r="L4" s="21">
         <v>0.15</v>
       </c>
-      <c r="M4" s="23">
-        <v>0</v>
-      </c>
-      <c r="N4" s="23">
-        <v>0</v>
-      </c>
-      <c r="O4" s="23">
-        <v>0</v>
-      </c>
-      <c r="P4" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="23">
+      <c r="M4" s="17">
+        <v>0</v>
+      </c>
+      <c r="N4" s="17">
+        <v>0</v>
+      </c>
+      <c r="O4" s="17">
+        <v>0</v>
+      </c>
+      <c r="P4" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="17">
         <v>4</v>
       </c>
       <c r="R4" s="4">
@@ -1875,7 +1680,7 @@
       <c r="T4" s="4">
         <v>0</v>
       </c>
-      <c r="U4" s="21">
+      <c r="U4" s="15">
         <v>4</v>
       </c>
       <c r="V4" s="3">
@@ -1932,55 +1737,55 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="23">
+        <v>79</v>
+      </c>
+      <c r="C5" s="17">
         <v>4</v>
       </c>
-      <c r="D5" s="23">
-        <v>1</v>
-      </c>
-      <c r="E5" s="25">
-        <v>1</v>
-      </c>
-      <c r="F5" s="26">
+      <c r="D5" s="17">
+        <v>1</v>
+      </c>
+      <c r="E5" s="19">
+        <v>1</v>
+      </c>
+      <c r="F5" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G5" s="25">
-        <v>0</v>
-      </c>
-      <c r="H5" s="23">
-        <v>0</v>
-      </c>
-      <c r="I5" s="23">
-        <v>0</v>
-      </c>
-      <c r="J5" s="23">
+      <c r="G5" s="19">
+        <v>0</v>
+      </c>
+      <c r="H5" s="17">
+        <v>0</v>
+      </c>
+      <c r="I5" s="17">
+        <v>0</v>
+      </c>
+      <c r="J5" s="17">
         <v>4</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K5" s="21">
         <v>0.2</v>
       </c>
-      <c r="L5" s="27">
+      <c r="L5" s="21">
         <v>0.45</v>
       </c>
-      <c r="M5" s="23">
-        <v>0</v>
-      </c>
-      <c r="N5" s="23">
-        <v>0</v>
-      </c>
-      <c r="O5" s="23">
-        <v>0</v>
-      </c>
-      <c r="P5" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="23">
+      <c r="M5" s="17">
+        <v>0</v>
+      </c>
+      <c r="N5" s="17">
+        <v>0</v>
+      </c>
+      <c r="O5" s="17">
+        <v>0</v>
+      </c>
+      <c r="P5" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="17">
         <v>4</v>
       </c>
       <c r="R5" s="4">
@@ -1992,7 +1797,7 @@
       <c r="T5" s="4">
         <v>0</v>
       </c>
-      <c r="U5" s="21">
+      <c r="U5" s="15">
         <v>4</v>
       </c>
       <c r="V5" s="3">
@@ -2049,55 +1854,55 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="23">
+        <v>80</v>
+      </c>
+      <c r="C6" s="17">
         <v>5</v>
       </c>
-      <c r="D6" s="23">
-        <v>1</v>
-      </c>
-      <c r="E6" s="25">
-        <v>1</v>
-      </c>
-      <c r="F6" s="26">
+      <c r="D6" s="17">
+        <v>1</v>
+      </c>
+      <c r="E6" s="19">
+        <v>1</v>
+      </c>
+      <c r="F6" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G6" s="25">
-        <v>0</v>
-      </c>
-      <c r="H6" s="23">
-        <v>0</v>
-      </c>
-      <c r="I6" s="23">
-        <v>0</v>
-      </c>
-      <c r="J6" s="23">
-        <v>1</v>
-      </c>
-      <c r="K6" s="28">
+      <c r="G6" s="19">
+        <v>0</v>
+      </c>
+      <c r="H6" s="17">
+        <v>0</v>
+      </c>
+      <c r="I6" s="17">
+        <v>0</v>
+      </c>
+      <c r="J6" s="17">
+        <v>1</v>
+      </c>
+      <c r="K6" s="22">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="L6" s="27">
+      <c r="L6" s="21">
         <v>0.15</v>
       </c>
-      <c r="M6" s="23">
-        <v>0</v>
-      </c>
-      <c r="N6" s="23">
-        <v>0</v>
-      </c>
-      <c r="O6" s="23">
-        <v>0</v>
-      </c>
-      <c r="P6" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="23">
+      <c r="M6" s="17">
+        <v>0</v>
+      </c>
+      <c r="N6" s="17">
+        <v>0</v>
+      </c>
+      <c r="O6" s="17">
+        <v>0</v>
+      </c>
+      <c r="P6" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="17">
         <v>4</v>
       </c>
       <c r="R6" s="4">
@@ -2109,7 +1914,7 @@
       <c r="T6" s="4">
         <v>0</v>
       </c>
-      <c r="U6" s="21">
+      <c r="U6" s="15">
         <v>4</v>
       </c>
       <c r="V6" s="3">
@@ -2166,55 +1971,55 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="23">
+        <v>81</v>
+      </c>
+      <c r="C7" s="17">
         <v>6</v>
       </c>
-      <c r="D7" s="23">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25">
-        <v>1</v>
-      </c>
-      <c r="F7" s="26">
+      <c r="D7" s="17">
+        <v>1</v>
+      </c>
+      <c r="E7" s="19">
+        <v>1</v>
+      </c>
+      <c r="F7" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G7" s="25">
-        <v>0</v>
-      </c>
-      <c r="H7" s="23">
-        <v>0</v>
-      </c>
-      <c r="I7" s="23">
-        <v>0</v>
-      </c>
-      <c r="J7" s="23">
-        <v>1</v>
-      </c>
-      <c r="K7" s="27">
+      <c r="G7" s="19">
+        <v>0</v>
+      </c>
+      <c r="H7" s="17">
+        <v>0</v>
+      </c>
+      <c r="I7" s="17">
+        <v>0</v>
+      </c>
+      <c r="J7" s="17">
+        <v>1</v>
+      </c>
+      <c r="K7" s="21">
         <v>0.2</v>
       </c>
-      <c r="L7" s="27">
+      <c r="L7" s="21">
         <v>0.45</v>
       </c>
-      <c r="M7" s="23">
-        <v>0</v>
-      </c>
-      <c r="N7" s="23">
-        <v>0</v>
-      </c>
-      <c r="O7" s="23">
-        <v>0</v>
-      </c>
-      <c r="P7" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="23">
+      <c r="M7" s="17">
+        <v>0</v>
+      </c>
+      <c r="N7" s="17">
+        <v>0</v>
+      </c>
+      <c r="O7" s="17">
+        <v>0</v>
+      </c>
+      <c r="P7" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="17">
         <v>4</v>
       </c>
       <c r="R7" s="4">
@@ -2226,7 +2031,7 @@
       <c r="T7" s="4">
         <v>0</v>
       </c>
-      <c r="U7" s="21">
+      <c r="U7" s="15">
         <v>4</v>
       </c>
       <c r="V7" s="3">
@@ -2283,55 +2088,55 @@
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="23">
+        <v>82</v>
+      </c>
+      <c r="C8" s="17">
         <v>7</v>
       </c>
-      <c r="D8" s="23">
-        <v>1</v>
-      </c>
-      <c r="E8" s="25">
-        <v>1</v>
-      </c>
-      <c r="F8" s="26">
+      <c r="D8" s="17">
+        <v>1</v>
+      </c>
+      <c r="E8" s="19">
+        <v>1</v>
+      </c>
+      <c r="F8" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G8" s="25">
-        <v>0</v>
-      </c>
-      <c r="H8" s="23">
-        <v>0</v>
-      </c>
-      <c r="I8" s="23">
-        <v>0</v>
-      </c>
-      <c r="J8" s="23">
+      <c r="G8" s="19">
+        <v>0</v>
+      </c>
+      <c r="H8" s="17">
+        <v>0</v>
+      </c>
+      <c r="I8" s="17">
+        <v>0</v>
+      </c>
+      <c r="J8" s="17">
         <v>7</v>
       </c>
-      <c r="K8" s="27">
+      <c r="K8" s="21">
         <v>0.4</v>
       </c>
-      <c r="L8" s="27">
+      <c r="L8" s="21">
         <v>0.75</v>
       </c>
-      <c r="M8" s="23">
-        <v>0</v>
-      </c>
-      <c r="N8" s="23">
-        <v>0</v>
-      </c>
-      <c r="O8" s="23">
-        <v>0</v>
-      </c>
-      <c r="P8" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="23">
+      <c r="M8" s="17">
+        <v>0</v>
+      </c>
+      <c r="N8" s="17">
+        <v>0</v>
+      </c>
+      <c r="O8" s="17">
+        <v>0</v>
+      </c>
+      <c r="P8" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="17">
         <v>4.5</v>
       </c>
       <c r="R8" s="4">
@@ -2343,7 +2148,7 @@
       <c r="T8" s="4">
         <v>0</v>
       </c>
-      <c r="U8" s="21">
+      <c r="U8" s="15">
         <v>4.5</v>
       </c>
       <c r="V8" s="3">
@@ -2400,55 +2205,55 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="23">
+        <v>83</v>
+      </c>
+      <c r="C9" s="17">
         <v>8</v>
       </c>
-      <c r="D9" s="23">
-        <v>1</v>
-      </c>
-      <c r="E9" s="25">
-        <v>1</v>
-      </c>
-      <c r="F9" s="26">
+      <c r="D9" s="17">
+        <v>1</v>
+      </c>
+      <c r="E9" s="19">
+        <v>1</v>
+      </c>
+      <c r="F9" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G9" s="25">
-        <v>0</v>
-      </c>
-      <c r="H9" s="23">
-        <v>0</v>
-      </c>
-      <c r="I9" s="23">
-        <v>0</v>
-      </c>
-      <c r="J9" s="23">
+      <c r="G9" s="19">
+        <v>0</v>
+      </c>
+      <c r="H9" s="17">
+        <v>0</v>
+      </c>
+      <c r="I9" s="17">
+        <v>0</v>
+      </c>
+      <c r="J9" s="17">
         <v>4</v>
       </c>
-      <c r="K9" s="27">
+      <c r="K9" s="21">
         <v>0.4</v>
       </c>
-      <c r="L9" s="27">
+      <c r="L9" s="21">
         <v>0.75</v>
       </c>
-      <c r="M9" s="23">
-        <v>0</v>
-      </c>
-      <c r="N9" s="23">
-        <v>0</v>
-      </c>
-      <c r="O9" s="23">
-        <v>0</v>
-      </c>
-      <c r="P9" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="23">
+      <c r="M9" s="17">
+        <v>0</v>
+      </c>
+      <c r="N9" s="17">
+        <v>0</v>
+      </c>
+      <c r="O9" s="17">
+        <v>0</v>
+      </c>
+      <c r="P9" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="17">
         <v>4.5</v>
       </c>
       <c r="R9" s="4">
@@ -2460,7 +2265,7 @@
       <c r="T9" s="4">
         <v>0</v>
       </c>
-      <c r="U9" s="21">
+      <c r="U9" s="15">
         <v>4.5</v>
       </c>
       <c r="V9" s="3">
@@ -2517,55 +2322,55 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" s="23">
+        <v>84</v>
+      </c>
+      <c r="C10" s="17">
         <v>9</v>
       </c>
-      <c r="D10" s="23">
-        <v>1</v>
-      </c>
-      <c r="E10" s="25">
-        <v>1</v>
-      </c>
-      <c r="F10" s="26">
+      <c r="D10" s="17">
+        <v>1</v>
+      </c>
+      <c r="E10" s="19">
+        <v>1</v>
+      </c>
+      <c r="F10" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G10" s="25">
-        <v>0</v>
-      </c>
-      <c r="H10" s="23">
-        <v>0</v>
-      </c>
-      <c r="I10" s="23">
-        <v>0</v>
-      </c>
-      <c r="J10" s="23">
-        <v>1</v>
-      </c>
-      <c r="K10" s="27">
+      <c r="G10" s="19">
+        <v>0</v>
+      </c>
+      <c r="H10" s="17">
+        <v>0</v>
+      </c>
+      <c r="I10" s="17">
+        <v>0</v>
+      </c>
+      <c r="J10" s="17">
+        <v>1</v>
+      </c>
+      <c r="K10" s="21">
         <v>0.4</v>
       </c>
-      <c r="L10" s="27">
+      <c r="L10" s="21">
         <v>0.75</v>
       </c>
-      <c r="M10" s="23">
-        <v>0</v>
-      </c>
-      <c r="N10" s="23">
-        <v>0</v>
-      </c>
-      <c r="O10" s="23">
-        <v>0</v>
-      </c>
-      <c r="P10" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="23">
+      <c r="M10" s="17">
+        <v>0</v>
+      </c>
+      <c r="N10" s="17">
+        <v>0</v>
+      </c>
+      <c r="O10" s="17">
+        <v>0</v>
+      </c>
+      <c r="P10" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="17">
         <v>4.5</v>
       </c>
       <c r="R10" s="4">
@@ -2577,7 +2382,7 @@
       <c r="T10" s="4">
         <v>0</v>
       </c>
-      <c r="U10" s="21">
+      <c r="U10" s="15">
         <v>4.5</v>
       </c>
       <c r="V10" s="3">
@@ -2637,52 +2442,52 @@
         <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" s="23">
+        <v>106</v>
+      </c>
+      <c r="C11" s="17">
         <v>10</v>
       </c>
-      <c r="D11" s="23">
-        <v>1</v>
-      </c>
-      <c r="E11" s="25">
-        <v>1</v>
-      </c>
-      <c r="F11" s="26">
+      <c r="D11" s="17">
+        <v>1</v>
+      </c>
+      <c r="E11" s="19">
+        <v>1</v>
+      </c>
+      <c r="F11" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G11" s="25">
-        <v>0</v>
-      </c>
-      <c r="H11" s="23">
-        <v>0</v>
-      </c>
-      <c r="I11" s="23">
-        <v>0</v>
-      </c>
-      <c r="J11" s="23">
-        <v>0</v>
-      </c>
-      <c r="K11" s="23">
-        <v>0</v>
-      </c>
-      <c r="L11" s="23">
-        <v>0</v>
-      </c>
-      <c r="M11" s="23">
-        <v>0</v>
-      </c>
-      <c r="N11" s="23">
-        <v>1</v>
-      </c>
-      <c r="O11" s="23">
-        <v>0</v>
-      </c>
-      <c r="P11" s="28">
+      <c r="G11" s="19">
+        <v>0</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0</v>
+      </c>
+      <c r="I11" s="17">
+        <v>0</v>
+      </c>
+      <c r="J11" s="17">
+        <v>0</v>
+      </c>
+      <c r="K11" s="17">
+        <v>0</v>
+      </c>
+      <c r="L11" s="17">
+        <v>0</v>
+      </c>
+      <c r="M11" s="17">
+        <v>0</v>
+      </c>
+      <c r="N11" s="17">
+        <v>1</v>
+      </c>
+      <c r="O11" s="17">
+        <v>0</v>
+      </c>
+      <c r="P11" s="22">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="Q11" s="23">
+      <c r="Q11" s="17">
         <v>4.5</v>
       </c>
       <c r="R11" s="4">
@@ -2721,7 +2526,7 @@
       <c r="AC11" s="4">
         <v>0</v>
       </c>
-      <c r="AD11" s="21">
+      <c r="AD11" s="15">
         <v>4.5</v>
       </c>
       <c r="AE11" s="3">
@@ -2754,52 +2559,52 @@
         <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="23">
+        <v>107</v>
+      </c>
+      <c r="C12" s="17">
         <v>11</v>
       </c>
-      <c r="D12" s="23">
-        <v>1</v>
-      </c>
-      <c r="E12" s="25">
-        <v>1</v>
-      </c>
-      <c r="F12" s="26">
+      <c r="D12" s="17">
+        <v>1</v>
+      </c>
+      <c r="E12" s="19">
+        <v>1</v>
+      </c>
+      <c r="F12" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G12" s="25">
-        <v>0</v>
-      </c>
-      <c r="H12" s="23">
-        <v>0</v>
-      </c>
-      <c r="I12" s="23">
-        <v>0</v>
-      </c>
-      <c r="J12" s="23">
-        <v>0</v>
-      </c>
-      <c r="K12" s="23">
-        <v>0</v>
-      </c>
-      <c r="L12" s="23">
-        <v>0</v>
-      </c>
-      <c r="M12" s="23">
-        <v>1</v>
-      </c>
-      <c r="N12" s="23">
-        <v>0</v>
-      </c>
-      <c r="O12" s="23">
-        <v>0</v>
-      </c>
-      <c r="P12" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="23">
+      <c r="G12" s="19">
+        <v>0</v>
+      </c>
+      <c r="H12" s="17">
+        <v>0</v>
+      </c>
+      <c r="I12" s="17">
+        <v>0</v>
+      </c>
+      <c r="J12" s="17">
+        <v>0</v>
+      </c>
+      <c r="K12" s="17">
+        <v>0</v>
+      </c>
+      <c r="L12" s="17">
+        <v>0</v>
+      </c>
+      <c r="M12" s="17">
+        <v>1</v>
+      </c>
+      <c r="N12" s="17">
+        <v>0</v>
+      </c>
+      <c r="O12" s="17">
+        <v>0</v>
+      </c>
+      <c r="P12" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="17">
         <v>5</v>
       </c>
       <c r="R12" s="4">
@@ -2838,7 +2643,7 @@
       <c r="AC12" s="4">
         <v>0</v>
       </c>
-      <c r="AD12" s="21">
+      <c r="AD12" s="15">
         <v>5</v>
       </c>
       <c r="AE12" s="3">
@@ -2868,55 +2673,55 @@
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="23">
+        <v>85</v>
+      </c>
+      <c r="C13" s="17">
         <v>12</v>
       </c>
-      <c r="D13" s="23">
-        <v>1</v>
-      </c>
-      <c r="E13" s="25">
-        <v>1</v>
-      </c>
-      <c r="F13" s="26">
+      <c r="D13" s="17">
+        <v>1</v>
+      </c>
+      <c r="E13" s="19">
+        <v>1</v>
+      </c>
+      <c r="F13" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G13" s="25">
-        <v>0</v>
-      </c>
-      <c r="H13" s="23">
-        <v>0</v>
-      </c>
-      <c r="I13" s="23">
-        <v>0</v>
-      </c>
-      <c r="J13" s="23">
+      <c r="G13" s="19">
+        <v>0</v>
+      </c>
+      <c r="H13" s="17">
+        <v>0</v>
+      </c>
+      <c r="I13" s="17">
+        <v>0</v>
+      </c>
+      <c r="J13" s="17">
         <v>7</v>
       </c>
-      <c r="K13" s="27">
+      <c r="K13" s="21">
         <v>0.8</v>
       </c>
-      <c r="L13" s="27">
+      <c r="L13" s="21">
         <v>1.35</v>
       </c>
-      <c r="M13" s="23">
-        <v>0</v>
-      </c>
-      <c r="N13" s="23">
-        <v>0</v>
-      </c>
-      <c r="O13" s="23">
-        <v>0</v>
-      </c>
-      <c r="P13" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="23">
+      <c r="M13" s="17">
+        <v>0</v>
+      </c>
+      <c r="N13" s="17">
+        <v>0</v>
+      </c>
+      <c r="O13" s="17">
+        <v>0</v>
+      </c>
+      <c r="P13" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="17">
         <v>5</v>
       </c>
       <c r="R13" s="4">
@@ -2928,7 +2733,7 @@
       <c r="T13" s="4">
         <v>0</v>
       </c>
-      <c r="U13" s="21">
+      <c r="U13" s="15">
         <v>5</v>
       </c>
       <c r="V13" s="3">
@@ -2985,55 +2790,55 @@
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="23">
+        <v>86</v>
+      </c>
+      <c r="C14" s="17">
         <v>13</v>
       </c>
-      <c r="D14" s="23">
-        <v>1</v>
-      </c>
-      <c r="E14" s="25">
-        <v>1</v>
-      </c>
-      <c r="F14" s="26">
+      <c r="D14" s="17">
+        <v>1</v>
+      </c>
+      <c r="E14" s="19">
+        <v>1</v>
+      </c>
+      <c r="F14" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G14" s="25">
-        <v>0</v>
-      </c>
-      <c r="H14" s="23">
-        <v>0</v>
-      </c>
-      <c r="I14" s="23">
-        <v>0</v>
-      </c>
-      <c r="J14" s="23">
+      <c r="G14" s="19">
+        <v>0</v>
+      </c>
+      <c r="H14" s="17">
+        <v>0</v>
+      </c>
+      <c r="I14" s="17">
+        <v>0</v>
+      </c>
+      <c r="J14" s="17">
         <v>7</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="17">
         <v>0.85</v>
       </c>
-      <c r="L14" s="27">
+      <c r="L14" s="21">
         <v>1.35</v>
       </c>
-      <c r="M14" s="23">
-        <v>0</v>
-      </c>
-      <c r="N14" s="23">
-        <v>0</v>
-      </c>
-      <c r="O14" s="23">
-        <v>0</v>
-      </c>
-      <c r="P14" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="23">
+      <c r="M14" s="17">
+        <v>0</v>
+      </c>
+      <c r="N14" s="17">
+        <v>0</v>
+      </c>
+      <c r="O14" s="17">
+        <v>0</v>
+      </c>
+      <c r="P14" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="17">
         <v>5</v>
       </c>
       <c r="R14" s="4">
@@ -3045,7 +2850,7 @@
       <c r="T14" s="4">
         <v>0</v>
       </c>
-      <c r="U14" s="21">
+      <c r="U14" s="15">
         <v>5</v>
       </c>
       <c r="V14" s="3">
@@ -3102,55 +2907,55 @@
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="23">
+        <v>87</v>
+      </c>
+      <c r="C15" s="17">
         <v>14</v>
       </c>
-      <c r="D15" s="23">
-        <v>1</v>
-      </c>
-      <c r="E15" s="25">
-        <v>1</v>
-      </c>
-      <c r="F15" s="26">
+      <c r="D15" s="17">
+        <v>1</v>
+      </c>
+      <c r="E15" s="19">
+        <v>1</v>
+      </c>
+      <c r="F15" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G15" s="25">
-        <v>0</v>
-      </c>
-      <c r="H15" s="23">
-        <v>0</v>
-      </c>
-      <c r="I15" s="23">
-        <v>0</v>
-      </c>
-      <c r="J15" s="23">
+      <c r="G15" s="19">
+        <v>0</v>
+      </c>
+      <c r="H15" s="17">
+        <v>0</v>
+      </c>
+      <c r="I15" s="17">
+        <v>0</v>
+      </c>
+      <c r="J15" s="17">
         <v>4</v>
       </c>
-      <c r="K15" s="27">
+      <c r="K15" s="21">
         <v>0.8</v>
       </c>
-      <c r="L15" s="27">
+      <c r="L15" s="21">
         <v>1.35</v>
       </c>
-      <c r="M15" s="23">
-        <v>0</v>
-      </c>
-      <c r="N15" s="23">
-        <v>0</v>
-      </c>
-      <c r="O15" s="23">
-        <v>0</v>
-      </c>
-      <c r="P15" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="23">
+      <c r="M15" s="17">
+        <v>0</v>
+      </c>
+      <c r="N15" s="17">
+        <v>0</v>
+      </c>
+      <c r="O15" s="17">
+        <v>0</v>
+      </c>
+      <c r="P15" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="17">
         <v>5</v>
       </c>
       <c r="R15" s="4">
@@ -3162,7 +2967,7 @@
       <c r="T15" s="4">
         <v>0</v>
       </c>
-      <c r="U15" s="21">
+      <c r="U15" s="15">
         <v>5</v>
       </c>
       <c r="V15" s="3">
@@ -3219,55 +3024,55 @@
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16" s="23">
+        <v>88</v>
+      </c>
+      <c r="C16" s="17">
         <v>15</v>
       </c>
-      <c r="D16" s="23">
-        <v>1</v>
-      </c>
-      <c r="E16" s="25">
-        <v>1</v>
-      </c>
-      <c r="F16" s="26">
+      <c r="D16" s="17">
+        <v>1</v>
+      </c>
+      <c r="E16" s="19">
+        <v>1</v>
+      </c>
+      <c r="F16" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G16" s="25">
-        <v>0</v>
-      </c>
-      <c r="H16" s="23">
-        <v>0</v>
-      </c>
-      <c r="I16" s="23">
-        <v>0</v>
-      </c>
-      <c r="J16" s="23">
-        <v>1</v>
-      </c>
-      <c r="K16" s="27">
+      <c r="G16" s="19">
+        <v>0</v>
+      </c>
+      <c r="H16" s="17">
+        <v>0</v>
+      </c>
+      <c r="I16" s="17">
+        <v>0</v>
+      </c>
+      <c r="J16" s="17">
+        <v>1</v>
+      </c>
+      <c r="K16" s="21">
         <v>0.8</v>
       </c>
-      <c r="L16" s="27">
+      <c r="L16" s="21">
         <v>1.35</v>
       </c>
-      <c r="M16" s="23">
-        <v>0</v>
-      </c>
-      <c r="N16" s="23">
-        <v>0</v>
-      </c>
-      <c r="O16" s="23">
-        <v>0</v>
-      </c>
-      <c r="P16" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="23">
+      <c r="M16" s="17">
+        <v>0</v>
+      </c>
+      <c r="N16" s="17">
+        <v>0</v>
+      </c>
+      <c r="O16" s="17">
+        <v>0</v>
+      </c>
+      <c r="P16" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="17">
         <v>5</v>
       </c>
       <c r="R16" s="4">
@@ -3279,7 +3084,7 @@
       <c r="T16" s="4">
         <v>0</v>
       </c>
-      <c r="U16" s="21">
+      <c r="U16" s="15">
         <v>5</v>
       </c>
       <c r="V16" s="3">
@@ -3339,52 +3144,52 @@
         <v>37</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="23">
+        <v>104</v>
+      </c>
+      <c r="C17" s="17">
         <v>16</v>
       </c>
-      <c r="D17" s="23">
-        <v>1</v>
-      </c>
-      <c r="E17" s="25">
-        <v>1</v>
-      </c>
-      <c r="F17" s="26">
+      <c r="D17" s="17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="19">
+        <v>1</v>
+      </c>
+      <c r="F17" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G17" s="25">
-        <v>0</v>
-      </c>
-      <c r="H17" s="23">
-        <v>0</v>
-      </c>
-      <c r="I17" s="23">
-        <v>0</v>
-      </c>
-      <c r="J17" s="23">
-        <v>0</v>
-      </c>
-      <c r="K17" s="23">
-        <v>0</v>
-      </c>
-      <c r="L17" s="23">
-        <v>0</v>
-      </c>
-      <c r="M17" s="23">
-        <v>0</v>
-      </c>
-      <c r="N17" s="23">
-        <v>1</v>
-      </c>
-      <c r="O17" s="23">
-        <v>0</v>
-      </c>
-      <c r="P17" s="28">
+      <c r="G17" s="19">
+        <v>0</v>
+      </c>
+      <c r="H17" s="17">
+        <v>0</v>
+      </c>
+      <c r="I17" s="17">
+        <v>0</v>
+      </c>
+      <c r="J17" s="17">
+        <v>0</v>
+      </c>
+      <c r="K17" s="17">
+        <v>0</v>
+      </c>
+      <c r="L17" s="17">
+        <v>0</v>
+      </c>
+      <c r="M17" s="17">
+        <v>0</v>
+      </c>
+      <c r="N17" s="17">
+        <v>1</v>
+      </c>
+      <c r="O17" s="17">
+        <v>0</v>
+      </c>
+      <c r="P17" s="22">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="Q17" s="23">
+      <c r="Q17" s="17">
         <v>6.5</v>
       </c>
       <c r="R17" s="4">
@@ -3409,12 +3214,12 @@
         <v>4.5</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z17" s="1">
         <v>0</v>
       </c>
-      <c r="AA17" s="21">
+      <c r="AA17" s="15">
         <v>6.5</v>
       </c>
       <c r="AB17" s="6" t="s">
@@ -3456,52 +3261,52 @@
         <v>36</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C18" s="23">
+        <v>105</v>
+      </c>
+      <c r="C18" s="17">
         <v>17</v>
       </c>
-      <c r="D18" s="23">
-        <v>1</v>
-      </c>
-      <c r="E18" s="25">
+      <c r="D18" s="17">
+        <v>1</v>
+      </c>
+      <c r="E18" s="19">
         <v>0.7</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G18" s="25">
-        <v>0</v>
-      </c>
-      <c r="H18" s="23">
-        <v>0</v>
-      </c>
-      <c r="I18" s="23">
-        <v>0</v>
-      </c>
-      <c r="J18" s="23">
-        <v>0</v>
-      </c>
-      <c r="K18" s="23">
-        <v>0</v>
-      </c>
-      <c r="L18" s="23">
-        <v>0</v>
-      </c>
-      <c r="M18" s="23">
-        <v>0</v>
-      </c>
-      <c r="N18" s="23">
-        <v>0</v>
-      </c>
-      <c r="O18" s="23">
-        <v>1</v>
-      </c>
-      <c r="P18" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="23">
+      <c r="G18" s="19">
+        <v>0</v>
+      </c>
+      <c r="H18" s="17">
+        <v>0</v>
+      </c>
+      <c r="I18" s="17">
+        <v>0</v>
+      </c>
+      <c r="J18" s="17">
+        <v>0</v>
+      </c>
+      <c r="K18" s="17">
+        <v>0</v>
+      </c>
+      <c r="L18" s="17">
+        <v>0</v>
+      </c>
+      <c r="M18" s="17">
+        <v>0</v>
+      </c>
+      <c r="N18" s="17">
+        <v>0</v>
+      </c>
+      <c r="O18" s="17">
+        <v>1</v>
+      </c>
+      <c r="P18" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="17">
         <v>10</v>
       </c>
       <c r="R18" s="4">
@@ -3549,7 +3354,7 @@
       <c r="AF18" s="4">
         <v>0</v>
       </c>
-      <c r="AG18" s="21">
+      <c r="AG18" s="15">
         <v>10</v>
       </c>
       <c r="AH18" s="3">
@@ -3570,25 +3375,25 @@
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="23">
+        <v>98</v>
+      </c>
+      <c r="C19" s="17">
         <v>18</v>
       </c>
-      <c r="D19" s="23">
-        <v>1</v>
-      </c>
-      <c r="E19" s="25">
+      <c r="D19" s="17">
+        <v>1</v>
+      </c>
+      <c r="E19" s="19">
         <v>0.7</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="19">
         <v>0</v>
       </c>
       <c r="H19" s="7">
@@ -3657,7 +3462,7 @@
       <c r="AC19" s="4">
         <v>0</v>
       </c>
-      <c r="AD19" s="21">
+      <c r="AD19" s="15">
         <v>18</v>
       </c>
       <c r="AE19" s="3">
@@ -3687,25 +3492,25 @@
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="23">
+        <v>99</v>
+      </c>
+      <c r="C20" s="17">
         <v>19</v>
       </c>
-      <c r="D20" s="23">
-        <v>1</v>
-      </c>
-      <c r="E20" s="25">
+      <c r="D20" s="17">
+        <v>1</v>
+      </c>
+      <c r="E20" s="19">
         <v>0.7</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="19">
         <v>0</v>
       </c>
       <c r="H20" s="7">
@@ -3742,7 +3547,7 @@
         <v>3</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T20" s="2" t="s">
         <v>27</v>
@@ -3751,7 +3556,7 @@
         <v>6</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W20" s="1">
         <v>0</v>
@@ -3769,12 +3574,12 @@
         <v>14.5</v>
       </c>
       <c r="AB20" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AC20" s="4">
         <v>0</v>
       </c>
-      <c r="AD20" s="21">
+      <c r="AD20" s="15">
         <v>18</v>
       </c>
       <c r="AE20" s="3">
@@ -3804,55 +3609,55 @@
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="23">
+        <v>102</v>
+      </c>
+      <c r="C21" s="17">
         <v>20</v>
       </c>
-      <c r="D21" s="23">
-        <v>1</v>
-      </c>
-      <c r="E21" s="25">
-        <v>1</v>
-      </c>
-      <c r="F21" s="26">
+      <c r="D21" s="17">
+        <v>1</v>
+      </c>
+      <c r="E21" s="19">
+        <v>1</v>
+      </c>
+      <c r="F21" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="19">
         <v>-0.33</v>
       </c>
-      <c r="H21" s="23">
-        <v>0</v>
-      </c>
-      <c r="I21" s="23">
-        <v>0</v>
-      </c>
-      <c r="J21" s="23">
-        <v>0</v>
-      </c>
-      <c r="K21" s="23">
-        <v>0</v>
-      </c>
-      <c r="L21" s="23">
-        <v>0</v>
-      </c>
-      <c r="M21" s="23">
-        <v>0</v>
-      </c>
-      <c r="N21" s="23">
-        <v>1</v>
-      </c>
-      <c r="O21" s="23">
-        <v>0</v>
-      </c>
-      <c r="P21" s="28">
+      <c r="H21" s="17">
+        <v>0</v>
+      </c>
+      <c r="I21" s="17">
+        <v>0</v>
+      </c>
+      <c r="J21" s="17">
+        <v>0</v>
+      </c>
+      <c r="K21" s="17">
+        <v>0</v>
+      </c>
+      <c r="L21" s="17">
+        <v>0</v>
+      </c>
+      <c r="M21" s="17">
+        <v>0</v>
+      </c>
+      <c r="N21" s="17">
+        <v>1</v>
+      </c>
+      <c r="O21" s="17">
+        <v>0</v>
+      </c>
+      <c r="P21" s="22">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="Q21" s="23">
+      <c r="Q21" s="17">
         <v>30</v>
       </c>
       <c r="R21" s="4">
@@ -3877,7 +3682,7 @@
         <v>17</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Z21" s="1">
         <v>0</v>
@@ -3891,7 +3696,7 @@
       <c r="AC21" s="4">
         <v>0</v>
       </c>
-      <c r="AD21" s="21">
+      <c r="AD21" s="15">
         <v>30</v>
       </c>
       <c r="AE21" s="3">
@@ -3921,55 +3726,55 @@
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C22" s="23">
+        <v>103</v>
+      </c>
+      <c r="C22" s="17">
         <v>21</v>
       </c>
-      <c r="D22" s="23">
-        <v>1</v>
-      </c>
-      <c r="E22" s="25">
-        <v>1</v>
-      </c>
-      <c r="F22" s="26">
+      <c r="D22" s="17">
+        <v>1</v>
+      </c>
+      <c r="E22" s="19">
+        <v>1</v>
+      </c>
+      <c r="F22" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="19">
         <v>0.33</v>
       </c>
-      <c r="H22" s="23">
-        <v>0</v>
-      </c>
-      <c r="I22" s="23">
-        <v>0</v>
-      </c>
-      <c r="J22" s="23">
-        <v>0</v>
-      </c>
-      <c r="K22" s="23">
-        <v>0</v>
-      </c>
-      <c r="L22" s="23">
-        <v>0</v>
-      </c>
-      <c r="M22" s="23">
-        <v>0</v>
-      </c>
-      <c r="N22" s="23">
-        <v>1</v>
-      </c>
-      <c r="O22" s="23">
-        <v>0</v>
-      </c>
-      <c r="P22" s="28">
+      <c r="H22" s="17">
+        <v>0</v>
+      </c>
+      <c r="I22" s="17">
+        <v>0</v>
+      </c>
+      <c r="J22" s="17">
+        <v>0</v>
+      </c>
+      <c r="K22" s="17">
+        <v>0</v>
+      </c>
+      <c r="L22" s="17">
+        <v>0</v>
+      </c>
+      <c r="M22" s="17">
+        <v>0</v>
+      </c>
+      <c r="N22" s="17">
+        <v>1</v>
+      </c>
+      <c r="O22" s="17">
+        <v>0</v>
+      </c>
+      <c r="P22" s="22">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="Q22" s="23">
+      <c r="Q22" s="17">
         <v>30</v>
       </c>
       <c r="R22" s="4">
@@ -4008,7 +3813,7 @@
       <c r="AC22" s="4">
         <v>0</v>
       </c>
-      <c r="AD22" s="21">
+      <c r="AD22" s="15">
         <v>30</v>
       </c>
       <c r="AE22" s="3">
@@ -4041,58 +3846,58 @@
         <v>40</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="23">
+        <v>96</v>
+      </c>
+      <c r="C23" s="17">
         <v>22</v>
       </c>
-      <c r="D23" s="23">
-        <v>1</v>
-      </c>
-      <c r="E23" s="25">
-        <v>1</v>
-      </c>
-      <c r="F23" s="29">
+      <c r="D23" s="17">
+        <v>1</v>
+      </c>
+      <c r="E23" s="19">
+        <v>1</v>
+      </c>
+      <c r="F23" s="23">
         <f>Input!H2</f>
         <v>1</v>
       </c>
-      <c r="G23" s="25">
-        <v>1</v>
-      </c>
-      <c r="H23" s="23">
-        <v>0</v>
-      </c>
-      <c r="I23" s="23">
-        <v>0</v>
-      </c>
-      <c r="J23" s="23">
-        <v>0</v>
-      </c>
-      <c r="K23" s="23">
-        <v>0</v>
-      </c>
-      <c r="L23" s="23">
-        <v>0</v>
-      </c>
-      <c r="M23" s="23">
-        <v>0</v>
-      </c>
-      <c r="N23" s="23">
-        <v>1</v>
-      </c>
-      <c r="O23" s="23">
-        <v>0</v>
-      </c>
-      <c r="P23" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="23">
+      <c r="G23" s="19">
+        <v>1</v>
+      </c>
+      <c r="H23" s="17">
+        <v>0</v>
+      </c>
+      <c r="I23" s="17">
+        <v>0</v>
+      </c>
+      <c r="J23" s="17">
+        <v>0</v>
+      </c>
+      <c r="K23" s="17">
+        <v>0</v>
+      </c>
+      <c r="L23" s="17">
+        <v>0</v>
+      </c>
+      <c r="M23" s="17">
+        <v>0</v>
+      </c>
+      <c r="N23" s="17">
+        <v>1</v>
+      </c>
+      <c r="O23" s="17">
+        <v>0</v>
+      </c>
+      <c r="P23" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="17">
         <v>52</v>
       </c>
       <c r="R23" s="4">
         <v>3</v>
       </c>
-      <c r="S23" s="34">
+      <c r="S23" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) + 0.025</f>
         <v>1.0316739272428239</v>
       </c>
@@ -4102,7 +3907,7 @@
       <c r="U23" s="1">
         <v>10</v>
       </c>
-      <c r="V23" s="34">
+      <c r="V23" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) - 0.025</f>
         <v>0.98167392724282398</v>
       </c>
@@ -4112,7 +3917,7 @@
       <c r="X23" s="1">
         <v>17</v>
       </c>
-      <c r="Y23" s="34">
+      <c r="Y23" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2)</f>
         <v>1.006673927242824</v>
       </c>
@@ -4122,7 +3927,7 @@
       <c r="AA23" s="1">
         <v>24</v>
       </c>
-      <c r="AB23" s="34">
+      <c r="AB23" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) + 0.05</f>
         <v>1.0566739272428241</v>
       </c>
@@ -4132,7 +3937,7 @@
       <c r="AD23" s="4">
         <v>31</v>
       </c>
-      <c r="AE23" s="34">
+      <c r="AE23" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2)</f>
         <v>1.006673927242824</v>
       </c>
@@ -4142,7 +3947,7 @@
       <c r="AG23" s="1">
         <v>38</v>
       </c>
-      <c r="AH23" s="34">
+      <c r="AH23" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) - 0.05</f>
         <v>0.95667392724282396</v>
       </c>
@@ -4152,7 +3957,7 @@
       <c r="AJ23" s="1">
         <v>45</v>
       </c>
-      <c r="AK23" s="34">
+      <c r="AK23" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2)</f>
         <v>1.006673927242824</v>
       </c>
@@ -4162,25 +3967,25 @@
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="23">
+        <v>93</v>
+      </c>
+      <c r="C24" s="17">
         <v>23</v>
       </c>
-      <c r="D24" s="23">
-        <v>1</v>
-      </c>
-      <c r="E24" s="25">
+      <c r="D24" s="17">
+        <v>1</v>
+      </c>
+      <c r="E24" s="19">
         <v>0.7</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="19">
         <v>0</v>
       </c>
       <c r="H24" s="7">
@@ -4210,7 +4015,7 @@
       <c r="P24" s="7">
         <v>1</v>
       </c>
-      <c r="Q24" s="12">
+      <c r="Q24" s="8">
         <v>80</v>
       </c>
       <c r="R24" s="4">
@@ -4222,7 +4027,7 @@
       <c r="T24" s="1">
         <v>0</v>
       </c>
-      <c r="U24" s="20">
+      <c r="U24" s="14">
         <v>80</v>
       </c>
       <c r="V24" s="3">
@@ -4279,25 +4084,25 @@
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="23">
+        <v>90</v>
+      </c>
+      <c r="C25" s="17">
         <v>24</v>
       </c>
-      <c r="D25" s="23">
-        <v>1</v>
-      </c>
-      <c r="E25" s="25">
+      <c r="D25" s="17">
+        <v>1</v>
+      </c>
+      <c r="E25" s="19">
         <v>0.5</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F25" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="19">
         <v>0</v>
       </c>
       <c r="H25" s="7">
@@ -4327,7 +4132,7 @@
       <c r="P25" s="7">
         <v>1</v>
       </c>
-      <c r="Q25" s="12">
+      <c r="Q25" s="8">
         <v>80</v>
       </c>
       <c r="R25" s="4">
@@ -4339,7 +4144,7 @@
       <c r="T25" s="1">
         <v>0</v>
       </c>
-      <c r="U25" s="20">
+      <c r="U25" s="14">
         <v>80</v>
       </c>
       <c r="V25" s="3">
@@ -4393,7 +4198,7 @@
       <c r="AL25" s="3">
         <v>0</v>
       </c>
-      <c r="AQ25" s="34">
+      <c r="AQ25" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) + 0.025</f>
         <v>1.0316739272428239</v>
       </c>
@@ -4403,52 +4208,52 @@
         <v>35</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="23">
+        <v>100</v>
+      </c>
+      <c r="C26" s="17">
         <v>25</v>
       </c>
-      <c r="D26" s="23">
-        <v>1</v>
-      </c>
-      <c r="E26" s="25">
+      <c r="D26" s="17">
+        <v>1</v>
+      </c>
+      <c r="E26" s="19">
         <v>0.7</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G26" s="25">
-        <v>0</v>
-      </c>
-      <c r="H26" s="23">
-        <v>0</v>
-      </c>
-      <c r="I26" s="23">
-        <v>0</v>
-      </c>
-      <c r="J26" s="23">
-        <v>0</v>
-      </c>
-      <c r="K26" s="23">
-        <v>0</v>
-      </c>
-      <c r="L26" s="23">
-        <v>0</v>
-      </c>
-      <c r="M26" s="23">
-        <v>0</v>
-      </c>
-      <c r="N26" s="23">
-        <v>0</v>
-      </c>
-      <c r="O26" s="23">
-        <v>1</v>
-      </c>
-      <c r="P26" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="23">
+      <c r="G26" s="19">
+        <v>0</v>
+      </c>
+      <c r="H26" s="17">
+        <v>0</v>
+      </c>
+      <c r="I26" s="17">
+        <v>0</v>
+      </c>
+      <c r="J26" s="17">
+        <v>0</v>
+      </c>
+      <c r="K26" s="17">
+        <v>0</v>
+      </c>
+      <c r="L26" s="17">
+        <v>0</v>
+      </c>
+      <c r="M26" s="17">
+        <v>0</v>
+      </c>
+      <c r="N26" s="17">
+        <v>0</v>
+      </c>
+      <c r="O26" s="17">
+        <v>1</v>
+      </c>
+      <c r="P26" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="17">
         <v>80</v>
       </c>
       <c r="R26" s="4">
@@ -4473,7 +4278,7 @@
         <v>42</v>
       </c>
       <c r="Y26" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z26" s="1">
         <v>0</v>
@@ -4487,7 +4292,7 @@
       <c r="AC26" s="4">
         <v>0</v>
       </c>
-      <c r="AD26" s="21">
+      <c r="AD26" s="15">
         <v>80</v>
       </c>
       <c r="AE26" s="3">
@@ -4520,52 +4325,52 @@
         <v>39</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="23">
+        <v>101</v>
+      </c>
+      <c r="C27" s="17">
         <v>26</v>
       </c>
-      <c r="D27" s="23">
-        <v>1</v>
-      </c>
-      <c r="E27" s="25">
+      <c r="D27" s="17">
+        <v>1</v>
+      </c>
+      <c r="E27" s="19">
         <v>0.7</v>
       </c>
-      <c r="F27" s="26">
+      <c r="F27" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G27" s="25">
-        <v>0</v>
-      </c>
-      <c r="H27" s="23">
-        <v>0</v>
-      </c>
-      <c r="I27" s="23">
-        <v>0</v>
-      </c>
-      <c r="J27" s="23">
-        <v>0</v>
-      </c>
-      <c r="K27" s="23">
-        <v>0</v>
-      </c>
-      <c r="L27" s="23">
-        <v>0</v>
-      </c>
-      <c r="M27" s="23">
-        <v>0</v>
-      </c>
-      <c r="N27" s="23">
-        <v>0</v>
-      </c>
-      <c r="O27" s="23">
-        <v>1</v>
-      </c>
-      <c r="P27" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="23">
+      <c r="G27" s="19">
+        <v>0</v>
+      </c>
+      <c r="H27" s="17">
+        <v>0</v>
+      </c>
+      <c r="I27" s="17">
+        <v>0</v>
+      </c>
+      <c r="J27" s="17">
+        <v>0</v>
+      </c>
+      <c r="K27" s="17">
+        <v>0</v>
+      </c>
+      <c r="L27" s="17">
+        <v>0</v>
+      </c>
+      <c r="M27" s="17">
+        <v>0</v>
+      </c>
+      <c r="N27" s="17">
+        <v>0</v>
+      </c>
+      <c r="O27" s="17">
+        <v>1</v>
+      </c>
+      <c r="P27" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="17">
         <v>80</v>
       </c>
       <c r="R27" s="4">
@@ -4590,7 +4395,7 @@
         <v>42</v>
       </c>
       <c r="Y27" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z27" s="1">
         <v>0</v>
@@ -4604,7 +4409,7 @@
       <c r="AC27" s="4">
         <v>0</v>
       </c>
-      <c r="AD27" s="21">
+      <c r="AD27" s="15">
         <v>80</v>
       </c>
       <c r="AE27" s="3">
@@ -4634,25 +4439,25 @@
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C28" s="23">
+        <v>92</v>
+      </c>
+      <c r="C28" s="17">
         <v>27</v>
       </c>
-      <c r="D28" s="23">
-        <v>1</v>
-      </c>
-      <c r="E28" s="25">
-        <v>1</v>
-      </c>
-      <c r="F28" s="26">
+      <c r="D28" s="17">
+        <v>1</v>
+      </c>
+      <c r="E28" s="19">
+        <v>1</v>
+      </c>
+      <c r="F28" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="19">
         <v>0</v>
       </c>
       <c r="H28" s="7">
@@ -4682,7 +4487,7 @@
       <c r="P28" s="7">
         <v>1</v>
       </c>
-      <c r="Q28" s="12">
+      <c r="Q28" s="8">
         <v>100</v>
       </c>
       <c r="R28" s="4">
@@ -4694,7 +4499,7 @@
       <c r="T28" s="1">
         <v>0</v>
       </c>
-      <c r="U28" s="20">
+      <c r="U28" s="14">
         <v>100</v>
       </c>
       <c r="V28" s="3">
@@ -4751,25 +4556,25 @@
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="23">
+        <v>91</v>
+      </c>
+      <c r="C29" s="17">
         <v>28</v>
       </c>
-      <c r="D29" s="23">
-        <v>1</v>
-      </c>
-      <c r="E29" s="25">
+      <c r="D29" s="17">
+        <v>1</v>
+      </c>
+      <c r="E29" s="19">
         <v>0.7</v>
       </c>
-      <c r="F29" s="26">
+      <c r="F29" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G29" s="25">
+      <c r="G29" s="19">
         <v>0</v>
       </c>
       <c r="H29" s="7">
@@ -4799,7 +4604,7 @@
       <c r="P29" s="7">
         <v>1</v>
       </c>
-      <c r="Q29" s="12">
+      <c r="Q29" s="8">
         <v>100</v>
       </c>
       <c r="R29" s="4">
@@ -4811,7 +4616,7 @@
       <c r="T29" s="1">
         <v>0</v>
       </c>
-      <c r="U29" s="20">
+      <c r="U29" s="14">
         <v>100</v>
       </c>
       <c r="V29" s="3">
@@ -4871,22 +4676,22 @@
         <v>41</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C30" s="23">
+        <v>97</v>
+      </c>
+      <c r="C30" s="17">
         <v>29</v>
       </c>
-      <c r="D30" s="23">
-        <v>1</v>
-      </c>
-      <c r="E30" s="25">
+      <c r="D30" s="17">
+        <v>1</v>
+      </c>
+      <c r="E30" s="19">
         <v>0.3</v>
       </c>
-      <c r="F30" s="29">
+      <c r="F30" s="23">
         <f>Input!I2</f>
         <v>2</v>
       </c>
-      <c r="G30" s="25">
+      <c r="G30" s="19">
         <v>0.99</v>
       </c>
       <c r="H30" s="7">
@@ -4955,7 +4760,7 @@
       <c r="AC30" s="1">
         <v>0</v>
       </c>
-      <c r="AD30" s="21">
+      <c r="AD30" s="15">
         <v>140</v>
       </c>
       <c r="AE30" s="3">
@@ -4988,22 +4793,22 @@
         <v>38</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" s="23">
+        <v>95</v>
+      </c>
+      <c r="C31" s="17">
         <v>30</v>
       </c>
-      <c r="D31" s="23">
-        <v>1</v>
-      </c>
-      <c r="E31" s="25">
-        <v>1</v>
-      </c>
-      <c r="F31" s="26">
+      <c r="D31" s="17">
+        <v>1</v>
+      </c>
+      <c r="E31" s="19">
+        <v>1</v>
+      </c>
+      <c r="F31" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G31" s="25">
+      <c r="G31" s="19">
         <v>0</v>
       </c>
       <c r="H31" s="7">
@@ -5072,7 +4877,7 @@
       <c r="AC31" s="1">
         <v>0</v>
       </c>
-      <c r="AD31" s="21">
+      <c r="AD31" s="15">
         <v>145</v>
       </c>
       <c r="AE31" s="3">
@@ -5105,22 +4910,22 @@
         <v>38</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C32" s="23">
+        <v>94</v>
+      </c>
+      <c r="C32" s="17">
         <v>31</v>
       </c>
-      <c r="D32" s="23">
-        <v>1</v>
-      </c>
-      <c r="E32" s="25">
-        <v>1</v>
-      </c>
-      <c r="F32" s="26">
+      <c r="D32" s="17">
+        <v>1</v>
+      </c>
+      <c r="E32" s="19">
+        <v>1</v>
+      </c>
+      <c r="F32" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G32" s="25">
+      <c r="G32" s="19">
         <v>0</v>
       </c>
       <c r="H32" s="7">
@@ -5189,7 +4994,7 @@
       <c r="AC32" s="1">
         <v>0</v>
       </c>
-      <c r="AD32" s="21">
+      <c r="AD32" s="15">
         <v>145</v>
       </c>
       <c r="AE32" s="3">
@@ -5219,25 +5024,25 @@
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" s="23">
+        <v>89</v>
+      </c>
+      <c r="C33" s="17">
         <v>32</v>
       </c>
-      <c r="D33" s="23">
-        <v>1</v>
-      </c>
-      <c r="E33" s="25">
-        <v>0</v>
-      </c>
-      <c r="F33" s="26">
+      <c r="D33" s="17">
+        <v>1</v>
+      </c>
+      <c r="E33" s="19">
+        <v>0</v>
+      </c>
+      <c r="F33" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G33" s="25">
+      <c r="G33" s="19">
         <v>0</v>
       </c>
       <c r="H33" s="7">
@@ -5279,7 +5084,7 @@
       <c r="T33" s="1">
         <v>0</v>
       </c>
-      <c r="U33" s="21">
+      <c r="U33" s="15">
         <v>155</v>
       </c>
       <c r="V33" s="3">
@@ -5351,300 +5156,91 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E2 E4 E6 E8 E10 E12 E14 E16">
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3 E5 E7 E9 E11 E13 E15 E17">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="44.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="9">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9">
-        <v>0</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="16">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="9">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="9">
-        <v>3</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="9">
-        <v>4</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0.7</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
-        <v>5</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
-        <v>6</v>
-      </c>
-      <c r="C7" s="9">
-        <v>1</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="9">
-        <v>7</v>
-      </c>
-      <c r="C8" s="9">
-        <v>1</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="9">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="9">
-        <v>8</v>
-      </c>
-      <c r="C9" s="9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="9">
-        <v>-0.33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
-        <v>9</v>
-      </c>
-      <c r="C10" s="9">
-        <v>0.6</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="9">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="9">
-        <v>10</v>
-      </c>
-      <c r="C11" s="10">
-        <v>0.6</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="9">
-        <v>-0.33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="9">
-        <v>11</v>
-      </c>
-      <c r="C12" s="10">
-        <v>0.3</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="9">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="9">
-        <v>12</v>
-      </c>
-      <c r="C13" s="10">
-        <v>0.3</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="9">
-        <v>-0.33</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C2:C13">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -5652,143 +5248,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="5" width="48.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>133</v>
-      </c>
-      <c r="D13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>138</v>
-      </c>
-      <c r="D15" t="s">
-        <v>125</v>
-      </c>
-      <c r="E15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>126</v>
-      </c>
-      <c r="E16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>127</v>
-      </c>
-      <c r="E17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>124</v>
-      </c>
-      <c r="E18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>140</v>
-      </c>
-      <c r="E19" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>141</v>
-      </c>
-      <c r="E20" t="s">
-        <v>143</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "'Balance' and 'PSCAD compilers' tabs removed"
This reverts commit dd34e92515c6cf11fba34ed54458c7a7e441aa3e.
</commit_message>
<xml_diff>
--- a/PSCAD/DK1_DSO_D/TestCases.xlsx
+++ b/PSCAD/DK1_DSO_D/TestCases.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\energinet.local\endk_funktion\Projekter\EffektGruppen\13_Medarbejdermapper\CVL\PP-MTB\PSCAD\DK1_DSO_D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MKT.ENERGINET\Desktop\PP-MTB-Alpha\PP-MTB PSCAD\DK1_DSO_D\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="350"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="350"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="2" r:id="rId1"/>
     <sheet name="Cases" sheetId="1" r:id="rId2"/>
+    <sheet name="Balance" sheetId="3" r:id="rId3"/>
+    <sheet name="PSCAD Compliers" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Input!$A$1:$M$2</definedName>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="149">
   <si>
     <t>PrefCtrl</t>
   </si>
@@ -169,6 +171,9 @@
     <t>0</t>
   </si>
   <si>
+    <t>Balance</t>
+  </si>
+  <si>
     <t>P0</t>
   </si>
   <si>
@@ -259,12 +264,25 @@
     <t>Qmode_PF: Power factor control</t>
   </si>
   <si>
+    <t>Additional information:
+An overview of all the balances tested</t>
+  </si>
+  <si>
     <t>Qmode</t>
   </si>
   <si>
     <t>InitValue</t>
   </si>
   <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>PF</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
     <t>TestType</t>
   </si>
   <si>
@@ -397,10 +415,139 @@
     <t>TotalCases</t>
   </si>
   <si>
+    <t>Intel(R) Visual Fortran Compiler XE 12.1.7.371</t>
+  </si>
+  <si>
+    <t>GFortran 4.6.2</t>
+  </si>
+  <si>
+    <t>GFortran 8.1</t>
+  </si>
+  <si>
+    <t>GFortran 8.1 (64-bit)</t>
+  </si>
+  <si>
     <t>Intel(R) Visual Fortran Compiler XE 15.0.1.148</t>
   </si>
   <si>
+    <t>Intel(R) Visual Fortran Compiler XE 15.0.1.148 (64-bit)</t>
+  </si>
+  <si>
+    <t>Intel(R) Visual Fortran Compiler XE 15.0.5.280</t>
+  </si>
+  <si>
+    <t>Intel(R) Visual Fortran Compiler XE 15.0.5.280 (64-bit)</t>
+  </si>
+  <si>
     <t>Note:</t>
+  </si>
+  <si>
+    <t>Servers:</t>
+  </si>
+  <si>
+    <t>X0133P01</t>
+  </si>
+  <si>
+    <t>Y0133P03</t>
+  </si>
+  <si>
+    <t>Y0133P01</t>
+  </si>
+  <si>
+    <t>Y0133P02</t>
+  </si>
+  <si>
+    <t>Compliers:</t>
+  </si>
+  <si>
+    <t>The compliers are different on different servers at Energinet.</t>
+  </si>
+  <si>
+    <r>
+      <t>Intel(R) Visual Fortran Compiler XE 15.0.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5.280</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Intel(R) Visual Fortran Compiler XE 15.0.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5.280</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (64-bit)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Intel(R) Visual Fortran Compiler XE 15.0.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.148</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Intel(R) Visual Fortran Compiler XE 15.0.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.148</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (64-bit)</t>
+    </r>
+  </si>
+  <si>
+    <t>See 'PSCAD Compliers' sheet for guidance</t>
   </si>
   <si>
     <t>Volley</t>
@@ -422,7 +569,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,6 +579,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -454,6 +608,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -521,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -544,10 +706,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -556,10 +730,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -577,7 +757,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -589,13 +769,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -612,7 +792,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1071,16 +1261,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="11" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="11" customWidth="1"/>
-    <col min="5" max="5" width="8" style="11" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="11"/>
+    <col min="2" max="2" width="6.42578125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="8" style="15" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="15"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
@@ -1090,64 +1282,64 @@
     <col min="13" max="13" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:14" s="14" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="F1" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="G1" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="H1" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="L1" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="N1" s="13" t="s">
+      <c r="I1" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="19" t="s">
         <v>121</v>
       </c>
+      <c r="L1" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="11">
+      <c r="B2" s="15">
         <v>10</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="15">
         <v>10</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="15">
         <v>62.5</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="15">
         <v>5</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="15">
         <v>15</v>
       </c>
       <c r="G2">
@@ -1160,10 +1352,10 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="K2" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="L2">
         <v>2</v>
@@ -1176,33 +1368,36 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G4" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="N4" s="26" t="s">
-        <v>122</v>
+      <c r="G4" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="K4" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
+      <c r="G5" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G6" s="26" t="s">
-        <v>70</v>
+      <c r="G6" s="32" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G7" s="26" t="s">
-        <v>71</v>
+      <c r="G7" s="32" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G8" s="26" t="s">
-        <v>72</v>
+      <c r="G8" s="32" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1216,7 +1411,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>#REF!</xm:f>
+            <xm:f>'PSCAD Compliers'!$A$1:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>K2</xm:sqref>
         </x14:dataValidation>
@@ -1273,67 +1468,67 @@
         <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="17" t="s">
+      <c r="G1" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q1" s="18" t="s">
+      <c r="P1" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q1" s="24" t="s">
         <v>8</v>
       </c>
       <c r="R1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="12" t="s">
         <v>15</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>16</v>
@@ -1342,7 +1537,7 @@
         <v>17</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Z1" s="4" t="s">
         <v>18</v>
@@ -1351,7 +1546,7 @@
         <v>19</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>20</v>
@@ -1360,7 +1555,7 @@
         <v>21</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>22</v>
@@ -1369,72 +1564,72 @@
         <v>30</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>31</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="17">
-        <v>1</v>
-      </c>
-      <c r="D2" s="17">
-        <v>1</v>
-      </c>
-      <c r="E2" s="19">
-        <v>1</v>
-      </c>
-      <c r="F2" s="20">
+        <v>81</v>
+      </c>
+      <c r="C2" s="23">
+        <v>1</v>
+      </c>
+      <c r="D2" s="23">
+        <v>1</v>
+      </c>
+      <c r="E2" s="25">
+        <v>1</v>
+      </c>
+      <c r="F2" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G2" s="19">
-        <v>0</v>
-      </c>
-      <c r="H2" s="17">
-        <v>0</v>
-      </c>
-      <c r="I2" s="17">
-        <v>0</v>
-      </c>
-      <c r="J2" s="17">
+      <c r="G2" s="25">
+        <v>0</v>
+      </c>
+      <c r="H2" s="23">
+        <v>0</v>
+      </c>
+      <c r="I2" s="23">
+        <v>0</v>
+      </c>
+      <c r="J2" s="23">
         <v>7</v>
       </c>
       <c r="K2" s="7">
         <v>0.01</v>
       </c>
-      <c r="L2" s="21">
+      <c r="L2" s="27">
         <v>0.15</v>
       </c>
-      <c r="M2" s="17">
-        <v>0</v>
-      </c>
-      <c r="N2" s="17">
-        <v>0</v>
-      </c>
-      <c r="O2" s="17">
-        <v>0</v>
-      </c>
-      <c r="P2" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="17">
+      <c r="M2" s="23">
+        <v>0</v>
+      </c>
+      <c r="N2" s="23">
+        <v>0</v>
+      </c>
+      <c r="O2" s="23">
+        <v>0</v>
+      </c>
+      <c r="P2" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="23">
         <v>4</v>
       </c>
       <c r="R2" s="4">
@@ -1446,7 +1641,7 @@
       <c r="T2" s="4">
         <v>0</v>
       </c>
-      <c r="U2" s="15">
+      <c r="U2" s="21">
         <v>4</v>
       </c>
       <c r="V2" s="3">
@@ -1503,55 +1698,55 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="17">
+        <v>82</v>
+      </c>
+      <c r="C3" s="23">
         <v>2</v>
       </c>
-      <c r="D3" s="17">
-        <v>1</v>
-      </c>
-      <c r="E3" s="19">
-        <v>1</v>
-      </c>
-      <c r="F3" s="20">
+      <c r="D3" s="23">
+        <v>1</v>
+      </c>
+      <c r="E3" s="25">
+        <v>1</v>
+      </c>
+      <c r="F3" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G3" s="19">
-        <v>0</v>
-      </c>
-      <c r="H3" s="17">
-        <v>0</v>
-      </c>
-      <c r="I3" s="17">
-        <v>0</v>
-      </c>
-      <c r="J3" s="17">
+      <c r="G3" s="25">
+        <v>0</v>
+      </c>
+      <c r="H3" s="23">
+        <v>0</v>
+      </c>
+      <c r="I3" s="23">
+        <v>0</v>
+      </c>
+      <c r="J3" s="23">
         <v>7</v>
       </c>
-      <c r="K3" s="21">
+      <c r="K3" s="27">
         <v>0.2</v>
       </c>
-      <c r="L3" s="21">
+      <c r="L3" s="27">
         <v>0.45</v>
       </c>
-      <c r="M3" s="17">
-        <v>0</v>
-      </c>
-      <c r="N3" s="17">
-        <v>0</v>
-      </c>
-      <c r="O3" s="17">
-        <v>0</v>
-      </c>
-      <c r="P3" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="17">
+      <c r="M3" s="23">
+        <v>0</v>
+      </c>
+      <c r="N3" s="23">
+        <v>0</v>
+      </c>
+      <c r="O3" s="23">
+        <v>0</v>
+      </c>
+      <c r="P3" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="23">
         <v>4</v>
       </c>
       <c r="R3" s="4">
@@ -1563,7 +1758,7 @@
       <c r="T3" s="4">
         <v>0</v>
       </c>
-      <c r="U3" s="15">
+      <c r="U3" s="21">
         <v>4</v>
       </c>
       <c r="V3" s="3">
@@ -1620,55 +1815,55 @@
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="17">
+        <v>83</v>
+      </c>
+      <c r="C4" s="23">
         <v>3</v>
       </c>
-      <c r="D4" s="17">
-        <v>1</v>
-      </c>
-      <c r="E4" s="19">
-        <v>1</v>
-      </c>
-      <c r="F4" s="20">
+      <c r="D4" s="23">
+        <v>1</v>
+      </c>
+      <c r="E4" s="25">
+        <v>1</v>
+      </c>
+      <c r="F4" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G4" s="19">
-        <v>0</v>
-      </c>
-      <c r="H4" s="17">
-        <v>0</v>
-      </c>
-      <c r="I4" s="17">
-        <v>0</v>
-      </c>
-      <c r="J4" s="17">
+      <c r="G4" s="25">
+        <v>0</v>
+      </c>
+      <c r="H4" s="23">
+        <v>0</v>
+      </c>
+      <c r="I4" s="23">
+        <v>0</v>
+      </c>
+      <c r="J4" s="23">
         <v>4</v>
       </c>
-      <c r="K4" s="22">
+      <c r="K4" s="28">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="L4" s="21">
+      <c r="L4" s="27">
         <v>0.15</v>
       </c>
-      <c r="M4" s="17">
-        <v>0</v>
-      </c>
-      <c r="N4" s="17">
-        <v>0</v>
-      </c>
-      <c r="O4" s="17">
-        <v>0</v>
-      </c>
-      <c r="P4" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="17">
+      <c r="M4" s="23">
+        <v>0</v>
+      </c>
+      <c r="N4" s="23">
+        <v>0</v>
+      </c>
+      <c r="O4" s="23">
+        <v>0</v>
+      </c>
+      <c r="P4" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="23">
         <v>4</v>
       </c>
       <c r="R4" s="4">
@@ -1680,7 +1875,7 @@
       <c r="T4" s="4">
         <v>0</v>
       </c>
-      <c r="U4" s="15">
+      <c r="U4" s="21">
         <v>4</v>
       </c>
       <c r="V4" s="3">
@@ -1737,55 +1932,55 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="17">
+        <v>84</v>
+      </c>
+      <c r="C5" s="23">
         <v>4</v>
       </c>
-      <c r="D5" s="17">
-        <v>1</v>
-      </c>
-      <c r="E5" s="19">
-        <v>1</v>
-      </c>
-      <c r="F5" s="20">
+      <c r="D5" s="23">
+        <v>1</v>
+      </c>
+      <c r="E5" s="25">
+        <v>1</v>
+      </c>
+      <c r="F5" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G5" s="19">
-        <v>0</v>
-      </c>
-      <c r="H5" s="17">
-        <v>0</v>
-      </c>
-      <c r="I5" s="17">
-        <v>0</v>
-      </c>
-      <c r="J5" s="17">
+      <c r="G5" s="25">
+        <v>0</v>
+      </c>
+      <c r="H5" s="23">
+        <v>0</v>
+      </c>
+      <c r="I5" s="23">
+        <v>0</v>
+      </c>
+      <c r="J5" s="23">
         <v>4</v>
       </c>
-      <c r="K5" s="21">
+      <c r="K5" s="27">
         <v>0.2</v>
       </c>
-      <c r="L5" s="21">
+      <c r="L5" s="27">
         <v>0.45</v>
       </c>
-      <c r="M5" s="17">
-        <v>0</v>
-      </c>
-      <c r="N5" s="17">
-        <v>0</v>
-      </c>
-      <c r="O5" s="17">
-        <v>0</v>
-      </c>
-      <c r="P5" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="17">
+      <c r="M5" s="23">
+        <v>0</v>
+      </c>
+      <c r="N5" s="23">
+        <v>0</v>
+      </c>
+      <c r="O5" s="23">
+        <v>0</v>
+      </c>
+      <c r="P5" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="23">
         <v>4</v>
       </c>
       <c r="R5" s="4">
@@ -1797,7 +1992,7 @@
       <c r="T5" s="4">
         <v>0</v>
       </c>
-      <c r="U5" s="15">
+      <c r="U5" s="21">
         <v>4</v>
       </c>
       <c r="V5" s="3">
@@ -1854,55 +2049,55 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="17">
+        <v>85</v>
+      </c>
+      <c r="C6" s="23">
         <v>5</v>
       </c>
-      <c r="D6" s="17">
-        <v>1</v>
-      </c>
-      <c r="E6" s="19">
-        <v>1</v>
-      </c>
-      <c r="F6" s="20">
+      <c r="D6" s="23">
+        <v>1</v>
+      </c>
+      <c r="E6" s="25">
+        <v>1</v>
+      </c>
+      <c r="F6" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G6" s="19">
-        <v>0</v>
-      </c>
-      <c r="H6" s="17">
-        <v>0</v>
-      </c>
-      <c r="I6" s="17">
-        <v>0</v>
-      </c>
-      <c r="J6" s="17">
-        <v>1</v>
-      </c>
-      <c r="K6" s="22">
+      <c r="G6" s="25">
+        <v>0</v>
+      </c>
+      <c r="H6" s="23">
+        <v>0</v>
+      </c>
+      <c r="I6" s="23">
+        <v>0</v>
+      </c>
+      <c r="J6" s="23">
+        <v>1</v>
+      </c>
+      <c r="K6" s="28">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6" s="27">
         <v>0.15</v>
       </c>
-      <c r="M6" s="17">
-        <v>0</v>
-      </c>
-      <c r="N6" s="17">
-        <v>0</v>
-      </c>
-      <c r="O6" s="17">
-        <v>0</v>
-      </c>
-      <c r="P6" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="17">
+      <c r="M6" s="23">
+        <v>0</v>
+      </c>
+      <c r="N6" s="23">
+        <v>0</v>
+      </c>
+      <c r="O6" s="23">
+        <v>0</v>
+      </c>
+      <c r="P6" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="23">
         <v>4</v>
       </c>
       <c r="R6" s="4">
@@ -1914,7 +2109,7 @@
       <c r="T6" s="4">
         <v>0</v>
       </c>
-      <c r="U6" s="15">
+      <c r="U6" s="21">
         <v>4</v>
       </c>
       <c r="V6" s="3">
@@ -1971,55 +2166,55 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="17">
+        <v>86</v>
+      </c>
+      <c r="C7" s="23">
         <v>6</v>
       </c>
-      <c r="D7" s="17">
-        <v>1</v>
-      </c>
-      <c r="E7" s="19">
-        <v>1</v>
-      </c>
-      <c r="F7" s="20">
+      <c r="D7" s="23">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25">
+        <v>1</v>
+      </c>
+      <c r="F7" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G7" s="19">
-        <v>0</v>
-      </c>
-      <c r="H7" s="17">
-        <v>0</v>
-      </c>
-      <c r="I7" s="17">
-        <v>0</v>
-      </c>
-      <c r="J7" s="17">
-        <v>1</v>
-      </c>
-      <c r="K7" s="21">
+      <c r="G7" s="25">
+        <v>0</v>
+      </c>
+      <c r="H7" s="23">
+        <v>0</v>
+      </c>
+      <c r="I7" s="23">
+        <v>0</v>
+      </c>
+      <c r="J7" s="23">
+        <v>1</v>
+      </c>
+      <c r="K7" s="27">
         <v>0.2</v>
       </c>
-      <c r="L7" s="21">
+      <c r="L7" s="27">
         <v>0.45</v>
       </c>
-      <c r="M7" s="17">
-        <v>0</v>
-      </c>
-      <c r="N7" s="17">
-        <v>0</v>
-      </c>
-      <c r="O7" s="17">
-        <v>0</v>
-      </c>
-      <c r="P7" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="17">
+      <c r="M7" s="23">
+        <v>0</v>
+      </c>
+      <c r="N7" s="23">
+        <v>0</v>
+      </c>
+      <c r="O7" s="23">
+        <v>0</v>
+      </c>
+      <c r="P7" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="23">
         <v>4</v>
       </c>
       <c r="R7" s="4">
@@ -2031,7 +2226,7 @@
       <c r="T7" s="4">
         <v>0</v>
       </c>
-      <c r="U7" s="15">
+      <c r="U7" s="21">
         <v>4</v>
       </c>
       <c r="V7" s="3">
@@ -2088,55 +2283,55 @@
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="17">
+        <v>87</v>
+      </c>
+      <c r="C8" s="23">
         <v>7</v>
       </c>
-      <c r="D8" s="17">
-        <v>1</v>
-      </c>
-      <c r="E8" s="19">
-        <v>1</v>
-      </c>
-      <c r="F8" s="20">
+      <c r="D8" s="23">
+        <v>1</v>
+      </c>
+      <c r="E8" s="25">
+        <v>1</v>
+      </c>
+      <c r="F8" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G8" s="19">
-        <v>0</v>
-      </c>
-      <c r="H8" s="17">
-        <v>0</v>
-      </c>
-      <c r="I8" s="17">
-        <v>0</v>
-      </c>
-      <c r="J8" s="17">
+      <c r="G8" s="25">
+        <v>0</v>
+      </c>
+      <c r="H8" s="23">
+        <v>0</v>
+      </c>
+      <c r="I8" s="23">
+        <v>0</v>
+      </c>
+      <c r="J8" s="23">
         <v>7</v>
       </c>
-      <c r="K8" s="21">
+      <c r="K8" s="27">
         <v>0.4</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="27">
         <v>0.75</v>
       </c>
-      <c r="M8" s="17">
-        <v>0</v>
-      </c>
-      <c r="N8" s="17">
-        <v>0</v>
-      </c>
-      <c r="O8" s="17">
-        <v>0</v>
-      </c>
-      <c r="P8" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="17">
+      <c r="M8" s="23">
+        <v>0</v>
+      </c>
+      <c r="N8" s="23">
+        <v>0</v>
+      </c>
+      <c r="O8" s="23">
+        <v>0</v>
+      </c>
+      <c r="P8" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="23">
         <v>4.5</v>
       </c>
       <c r="R8" s="4">
@@ -2148,7 +2343,7 @@
       <c r="T8" s="4">
         <v>0</v>
       </c>
-      <c r="U8" s="15">
+      <c r="U8" s="21">
         <v>4.5</v>
       </c>
       <c r="V8" s="3">
@@ -2205,55 +2400,55 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="17">
+        <v>88</v>
+      </c>
+      <c r="C9" s="23">
         <v>8</v>
       </c>
-      <c r="D9" s="17">
-        <v>1</v>
-      </c>
-      <c r="E9" s="19">
-        <v>1</v>
-      </c>
-      <c r="F9" s="20">
+      <c r="D9" s="23">
+        <v>1</v>
+      </c>
+      <c r="E9" s="25">
+        <v>1</v>
+      </c>
+      <c r="F9" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G9" s="19">
-        <v>0</v>
-      </c>
-      <c r="H9" s="17">
-        <v>0</v>
-      </c>
-      <c r="I9" s="17">
-        <v>0</v>
-      </c>
-      <c r="J9" s="17">
+      <c r="G9" s="25">
+        <v>0</v>
+      </c>
+      <c r="H9" s="23">
+        <v>0</v>
+      </c>
+      <c r="I9" s="23">
+        <v>0</v>
+      </c>
+      <c r="J9" s="23">
         <v>4</v>
       </c>
-      <c r="K9" s="21">
+      <c r="K9" s="27">
         <v>0.4</v>
       </c>
-      <c r="L9" s="21">
+      <c r="L9" s="27">
         <v>0.75</v>
       </c>
-      <c r="M9" s="17">
-        <v>0</v>
-      </c>
-      <c r="N9" s="17">
-        <v>0</v>
-      </c>
-      <c r="O9" s="17">
-        <v>0</v>
-      </c>
-      <c r="P9" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="17">
+      <c r="M9" s="23">
+        <v>0</v>
+      </c>
+      <c r="N9" s="23">
+        <v>0</v>
+      </c>
+      <c r="O9" s="23">
+        <v>0</v>
+      </c>
+      <c r="P9" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="23">
         <v>4.5</v>
       </c>
       <c r="R9" s="4">
@@ -2265,7 +2460,7 @@
       <c r="T9" s="4">
         <v>0</v>
       </c>
-      <c r="U9" s="15">
+      <c r="U9" s="21">
         <v>4.5</v>
       </c>
       <c r="V9" s="3">
@@ -2322,55 +2517,55 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="17">
+        <v>89</v>
+      </c>
+      <c r="C10" s="23">
         <v>9</v>
       </c>
-      <c r="D10" s="17">
-        <v>1</v>
-      </c>
-      <c r="E10" s="19">
-        <v>1</v>
-      </c>
-      <c r="F10" s="20">
+      <c r="D10" s="23">
+        <v>1</v>
+      </c>
+      <c r="E10" s="25">
+        <v>1</v>
+      </c>
+      <c r="F10" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G10" s="19">
-        <v>0</v>
-      </c>
-      <c r="H10" s="17">
-        <v>0</v>
-      </c>
-      <c r="I10" s="17">
-        <v>0</v>
-      </c>
-      <c r="J10" s="17">
-        <v>1</v>
-      </c>
-      <c r="K10" s="21">
+      <c r="G10" s="25">
+        <v>0</v>
+      </c>
+      <c r="H10" s="23">
+        <v>0</v>
+      </c>
+      <c r="I10" s="23">
+        <v>0</v>
+      </c>
+      <c r="J10" s="23">
+        <v>1</v>
+      </c>
+      <c r="K10" s="27">
         <v>0.4</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="27">
         <v>0.75</v>
       </c>
-      <c r="M10" s="17">
-        <v>0</v>
-      </c>
-      <c r="N10" s="17">
-        <v>0</v>
-      </c>
-      <c r="O10" s="17">
-        <v>0</v>
-      </c>
-      <c r="P10" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="17">
+      <c r="M10" s="23">
+        <v>0</v>
+      </c>
+      <c r="N10" s="23">
+        <v>0</v>
+      </c>
+      <c r="O10" s="23">
+        <v>0</v>
+      </c>
+      <c r="P10" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="23">
         <v>4.5</v>
       </c>
       <c r="R10" s="4">
@@ -2382,7 +2577,7 @@
       <c r="T10" s="4">
         <v>0</v>
       </c>
-      <c r="U10" s="15">
+      <c r="U10" s="21">
         <v>4.5</v>
       </c>
       <c r="V10" s="3">
@@ -2442,52 +2637,52 @@
         <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="17">
+        <v>111</v>
+      </c>
+      <c r="C11" s="23">
         <v>10</v>
       </c>
-      <c r="D11" s="17">
-        <v>1</v>
-      </c>
-      <c r="E11" s="19">
-        <v>1</v>
-      </c>
-      <c r="F11" s="20">
+      <c r="D11" s="23">
+        <v>1</v>
+      </c>
+      <c r="E11" s="25">
+        <v>1</v>
+      </c>
+      <c r="F11" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G11" s="19">
-        <v>0</v>
-      </c>
-      <c r="H11" s="17">
-        <v>0</v>
-      </c>
-      <c r="I11" s="17">
-        <v>0</v>
-      </c>
-      <c r="J11" s="17">
-        <v>0</v>
-      </c>
-      <c r="K11" s="17">
-        <v>0</v>
-      </c>
-      <c r="L11" s="17">
-        <v>0</v>
-      </c>
-      <c r="M11" s="17">
-        <v>0</v>
-      </c>
-      <c r="N11" s="17">
-        <v>1</v>
-      </c>
-      <c r="O11" s="17">
-        <v>0</v>
-      </c>
-      <c r="P11" s="22">
+      <c r="G11" s="25">
+        <v>0</v>
+      </c>
+      <c r="H11" s="23">
+        <v>0</v>
+      </c>
+      <c r="I11" s="23">
+        <v>0</v>
+      </c>
+      <c r="J11" s="23">
+        <v>0</v>
+      </c>
+      <c r="K11" s="23">
+        <v>0</v>
+      </c>
+      <c r="L11" s="23">
+        <v>0</v>
+      </c>
+      <c r="M11" s="23">
+        <v>0</v>
+      </c>
+      <c r="N11" s="23">
+        <v>1</v>
+      </c>
+      <c r="O11" s="23">
+        <v>0</v>
+      </c>
+      <c r="P11" s="28">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="Q11" s="17">
+      <c r="Q11" s="23">
         <v>4.5</v>
       </c>
       <c r="R11" s="4">
@@ -2526,7 +2721,7 @@
       <c r="AC11" s="4">
         <v>0</v>
       </c>
-      <c r="AD11" s="15">
+      <c r="AD11" s="21">
         <v>4.5</v>
       </c>
       <c r="AE11" s="3">
@@ -2559,52 +2754,52 @@
         <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="17">
+        <v>112</v>
+      </c>
+      <c r="C12" s="23">
         <v>11</v>
       </c>
-      <c r="D12" s="17">
-        <v>1</v>
-      </c>
-      <c r="E12" s="19">
-        <v>1</v>
-      </c>
-      <c r="F12" s="20">
+      <c r="D12" s="23">
+        <v>1</v>
+      </c>
+      <c r="E12" s="25">
+        <v>1</v>
+      </c>
+      <c r="F12" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G12" s="19">
-        <v>0</v>
-      </c>
-      <c r="H12" s="17">
-        <v>0</v>
-      </c>
-      <c r="I12" s="17">
-        <v>0</v>
-      </c>
-      <c r="J12" s="17">
-        <v>0</v>
-      </c>
-      <c r="K12" s="17">
-        <v>0</v>
-      </c>
-      <c r="L12" s="17">
-        <v>0</v>
-      </c>
-      <c r="M12" s="17">
-        <v>1</v>
-      </c>
-      <c r="N12" s="17">
-        <v>0</v>
-      </c>
-      <c r="O12" s="17">
-        <v>0</v>
-      </c>
-      <c r="P12" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="17">
+      <c r="G12" s="25">
+        <v>0</v>
+      </c>
+      <c r="H12" s="23">
+        <v>0</v>
+      </c>
+      <c r="I12" s="23">
+        <v>0</v>
+      </c>
+      <c r="J12" s="23">
+        <v>0</v>
+      </c>
+      <c r="K12" s="23">
+        <v>0</v>
+      </c>
+      <c r="L12" s="23">
+        <v>0</v>
+      </c>
+      <c r="M12" s="23">
+        <v>1</v>
+      </c>
+      <c r="N12" s="23">
+        <v>0</v>
+      </c>
+      <c r="O12" s="23">
+        <v>0</v>
+      </c>
+      <c r="P12" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="23">
         <v>5</v>
       </c>
       <c r="R12" s="4">
@@ -2643,7 +2838,7 @@
       <c r="AC12" s="4">
         <v>0</v>
       </c>
-      <c r="AD12" s="15">
+      <c r="AD12" s="21">
         <v>5</v>
       </c>
       <c r="AE12" s="3">
@@ -2673,55 +2868,55 @@
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="17">
+        <v>90</v>
+      </c>
+      <c r="C13" s="23">
         <v>12</v>
       </c>
-      <c r="D13" s="17">
-        <v>1</v>
-      </c>
-      <c r="E13" s="19">
-        <v>1</v>
-      </c>
-      <c r="F13" s="20">
+      <c r="D13" s="23">
+        <v>1</v>
+      </c>
+      <c r="E13" s="25">
+        <v>1</v>
+      </c>
+      <c r="F13" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G13" s="19">
-        <v>0</v>
-      </c>
-      <c r="H13" s="17">
-        <v>0</v>
-      </c>
-      <c r="I13" s="17">
-        <v>0</v>
-      </c>
-      <c r="J13" s="17">
+      <c r="G13" s="25">
+        <v>0</v>
+      </c>
+      <c r="H13" s="23">
+        <v>0</v>
+      </c>
+      <c r="I13" s="23">
+        <v>0</v>
+      </c>
+      <c r="J13" s="23">
         <v>7</v>
       </c>
-      <c r="K13" s="21">
+      <c r="K13" s="27">
         <v>0.8</v>
       </c>
-      <c r="L13" s="21">
+      <c r="L13" s="27">
         <v>1.35</v>
       </c>
-      <c r="M13" s="17">
-        <v>0</v>
-      </c>
-      <c r="N13" s="17">
-        <v>0</v>
-      </c>
-      <c r="O13" s="17">
-        <v>0</v>
-      </c>
-      <c r="P13" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="17">
+      <c r="M13" s="23">
+        <v>0</v>
+      </c>
+      <c r="N13" s="23">
+        <v>0</v>
+      </c>
+      <c r="O13" s="23">
+        <v>0</v>
+      </c>
+      <c r="P13" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="23">
         <v>5</v>
       </c>
       <c r="R13" s="4">
@@ -2733,7 +2928,7 @@
       <c r="T13" s="4">
         <v>0</v>
       </c>
-      <c r="U13" s="15">
+      <c r="U13" s="21">
         <v>5</v>
       </c>
       <c r="V13" s="3">
@@ -2790,55 +2985,55 @@
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="17">
+        <v>91</v>
+      </c>
+      <c r="C14" s="23">
         <v>13</v>
       </c>
-      <c r="D14" s="17">
-        <v>1</v>
-      </c>
-      <c r="E14" s="19">
-        <v>1</v>
-      </c>
-      <c r="F14" s="20">
+      <c r="D14" s="23">
+        <v>1</v>
+      </c>
+      <c r="E14" s="25">
+        <v>1</v>
+      </c>
+      <c r="F14" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G14" s="19">
-        <v>0</v>
-      </c>
-      <c r="H14" s="17">
-        <v>0</v>
-      </c>
-      <c r="I14" s="17">
-        <v>0</v>
-      </c>
-      <c r="J14" s="17">
+      <c r="G14" s="25">
+        <v>0</v>
+      </c>
+      <c r="H14" s="23">
+        <v>0</v>
+      </c>
+      <c r="I14" s="23">
+        <v>0</v>
+      </c>
+      <c r="J14" s="23">
         <v>7</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14" s="23">
         <v>0.85</v>
       </c>
-      <c r="L14" s="21">
+      <c r="L14" s="27">
         <v>1.35</v>
       </c>
-      <c r="M14" s="17">
-        <v>0</v>
-      </c>
-      <c r="N14" s="17">
-        <v>0</v>
-      </c>
-      <c r="O14" s="17">
-        <v>0</v>
-      </c>
-      <c r="P14" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="17">
+      <c r="M14" s="23">
+        <v>0</v>
+      </c>
+      <c r="N14" s="23">
+        <v>0</v>
+      </c>
+      <c r="O14" s="23">
+        <v>0</v>
+      </c>
+      <c r="P14" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="23">
         <v>5</v>
       </c>
       <c r="R14" s="4">
@@ -2850,7 +3045,7 @@
       <c r="T14" s="4">
         <v>0</v>
       </c>
-      <c r="U14" s="15">
+      <c r="U14" s="21">
         <v>5</v>
       </c>
       <c r="V14" s="3">
@@ -2907,55 +3102,55 @@
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="17">
+        <v>92</v>
+      </c>
+      <c r="C15" s="23">
         <v>14</v>
       </c>
-      <c r="D15" s="17">
-        <v>1</v>
-      </c>
-      <c r="E15" s="19">
-        <v>1</v>
-      </c>
-      <c r="F15" s="20">
+      <c r="D15" s="23">
+        <v>1</v>
+      </c>
+      <c r="E15" s="25">
+        <v>1</v>
+      </c>
+      <c r="F15" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G15" s="19">
-        <v>0</v>
-      </c>
-      <c r="H15" s="17">
-        <v>0</v>
-      </c>
-      <c r="I15" s="17">
-        <v>0</v>
-      </c>
-      <c r="J15" s="17">
+      <c r="G15" s="25">
+        <v>0</v>
+      </c>
+      <c r="H15" s="23">
+        <v>0</v>
+      </c>
+      <c r="I15" s="23">
+        <v>0</v>
+      </c>
+      <c r="J15" s="23">
         <v>4</v>
       </c>
-      <c r="K15" s="21">
+      <c r="K15" s="27">
         <v>0.8</v>
       </c>
-      <c r="L15" s="21">
+      <c r="L15" s="27">
         <v>1.35</v>
       </c>
-      <c r="M15" s="17">
-        <v>0</v>
-      </c>
-      <c r="N15" s="17">
-        <v>0</v>
-      </c>
-      <c r="O15" s="17">
-        <v>0</v>
-      </c>
-      <c r="P15" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="17">
+      <c r="M15" s="23">
+        <v>0</v>
+      </c>
+      <c r="N15" s="23">
+        <v>0</v>
+      </c>
+      <c r="O15" s="23">
+        <v>0</v>
+      </c>
+      <c r="P15" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="23">
         <v>5</v>
       </c>
       <c r="R15" s="4">
@@ -2967,7 +3162,7 @@
       <c r="T15" s="4">
         <v>0</v>
       </c>
-      <c r="U15" s="15">
+      <c r="U15" s="21">
         <v>5</v>
       </c>
       <c r="V15" s="3">
@@ -3024,55 +3219,55 @@
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="17">
+        <v>93</v>
+      </c>
+      <c r="C16" s="23">
         <v>15</v>
       </c>
-      <c r="D16" s="17">
-        <v>1</v>
-      </c>
-      <c r="E16" s="19">
-        <v>1</v>
-      </c>
-      <c r="F16" s="20">
+      <c r="D16" s="23">
+        <v>1</v>
+      </c>
+      <c r="E16" s="25">
+        <v>1</v>
+      </c>
+      <c r="F16" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G16" s="19">
-        <v>0</v>
-      </c>
-      <c r="H16" s="17">
-        <v>0</v>
-      </c>
-      <c r="I16" s="17">
-        <v>0</v>
-      </c>
-      <c r="J16" s="17">
-        <v>1</v>
-      </c>
-      <c r="K16" s="21">
+      <c r="G16" s="25">
+        <v>0</v>
+      </c>
+      <c r="H16" s="23">
+        <v>0</v>
+      </c>
+      <c r="I16" s="23">
+        <v>0</v>
+      </c>
+      <c r="J16" s="23">
+        <v>1</v>
+      </c>
+      <c r="K16" s="27">
         <v>0.8</v>
       </c>
-      <c r="L16" s="21">
+      <c r="L16" s="27">
         <v>1.35</v>
       </c>
-      <c r="M16" s="17">
-        <v>0</v>
-      </c>
-      <c r="N16" s="17">
-        <v>0</v>
-      </c>
-      <c r="O16" s="17">
-        <v>0</v>
-      </c>
-      <c r="P16" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="17">
+      <c r="M16" s="23">
+        <v>0</v>
+      </c>
+      <c r="N16" s="23">
+        <v>0</v>
+      </c>
+      <c r="O16" s="23">
+        <v>0</v>
+      </c>
+      <c r="P16" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="23">
         <v>5</v>
       </c>
       <c r="R16" s="4">
@@ -3084,7 +3279,7 @@
       <c r="T16" s="4">
         <v>0</v>
       </c>
-      <c r="U16" s="15">
+      <c r="U16" s="21">
         <v>5</v>
       </c>
       <c r="V16" s="3">
@@ -3144,52 +3339,52 @@
         <v>37</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="17">
+        <v>109</v>
+      </c>
+      <c r="C17" s="23">
         <v>16</v>
       </c>
-      <c r="D17" s="17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="19">
-        <v>1</v>
-      </c>
-      <c r="F17" s="20">
+      <c r="D17" s="23">
+        <v>1</v>
+      </c>
+      <c r="E17" s="25">
+        <v>1</v>
+      </c>
+      <c r="F17" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G17" s="19">
-        <v>0</v>
-      </c>
-      <c r="H17" s="17">
-        <v>0</v>
-      </c>
-      <c r="I17" s="17">
-        <v>0</v>
-      </c>
-      <c r="J17" s="17">
-        <v>0</v>
-      </c>
-      <c r="K17" s="17">
-        <v>0</v>
-      </c>
-      <c r="L17" s="17">
-        <v>0</v>
-      </c>
-      <c r="M17" s="17">
-        <v>0</v>
-      </c>
-      <c r="N17" s="17">
-        <v>1</v>
-      </c>
-      <c r="O17" s="17">
-        <v>0</v>
-      </c>
-      <c r="P17" s="22">
+      <c r="G17" s="25">
+        <v>0</v>
+      </c>
+      <c r="H17" s="23">
+        <v>0</v>
+      </c>
+      <c r="I17" s="23">
+        <v>0</v>
+      </c>
+      <c r="J17" s="23">
+        <v>0</v>
+      </c>
+      <c r="K17" s="23">
+        <v>0</v>
+      </c>
+      <c r="L17" s="23">
+        <v>0</v>
+      </c>
+      <c r="M17" s="23">
+        <v>0</v>
+      </c>
+      <c r="N17" s="23">
+        <v>1</v>
+      </c>
+      <c r="O17" s="23">
+        <v>0</v>
+      </c>
+      <c r="P17" s="28">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="Q17" s="17">
+      <c r="Q17" s="23">
         <v>6.5</v>
       </c>
       <c r="R17" s="4">
@@ -3214,12 +3409,12 @@
         <v>4.5</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Z17" s="1">
         <v>0</v>
       </c>
-      <c r="AA17" s="15">
+      <c r="AA17" s="21">
         <v>6.5</v>
       </c>
       <c r="AB17" s="6" t="s">
@@ -3261,52 +3456,52 @@
         <v>36</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="17">
+        <v>110</v>
+      </c>
+      <c r="C18" s="23">
         <v>17</v>
       </c>
-      <c r="D18" s="17">
-        <v>1</v>
-      </c>
-      <c r="E18" s="19">
+      <c r="D18" s="23">
+        <v>1</v>
+      </c>
+      <c r="E18" s="25">
         <v>0.7</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G18" s="19">
-        <v>0</v>
-      </c>
-      <c r="H18" s="17">
-        <v>0</v>
-      </c>
-      <c r="I18" s="17">
-        <v>0</v>
-      </c>
-      <c r="J18" s="17">
-        <v>0</v>
-      </c>
-      <c r="K18" s="17">
-        <v>0</v>
-      </c>
-      <c r="L18" s="17">
-        <v>0</v>
-      </c>
-      <c r="M18" s="17">
-        <v>0</v>
-      </c>
-      <c r="N18" s="17">
-        <v>0</v>
-      </c>
-      <c r="O18" s="17">
-        <v>1</v>
-      </c>
-      <c r="P18" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="17">
+      <c r="G18" s="25">
+        <v>0</v>
+      </c>
+      <c r="H18" s="23">
+        <v>0</v>
+      </c>
+      <c r="I18" s="23">
+        <v>0</v>
+      </c>
+      <c r="J18" s="23">
+        <v>0</v>
+      </c>
+      <c r="K18" s="23">
+        <v>0</v>
+      </c>
+      <c r="L18" s="23">
+        <v>0</v>
+      </c>
+      <c r="M18" s="23">
+        <v>0</v>
+      </c>
+      <c r="N18" s="23">
+        <v>0</v>
+      </c>
+      <c r="O18" s="23">
+        <v>1</v>
+      </c>
+      <c r="P18" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="23">
         <v>10</v>
       </c>
       <c r="R18" s="4">
@@ -3354,7 +3549,7 @@
       <c r="AF18" s="4">
         <v>0</v>
       </c>
-      <c r="AG18" s="15">
+      <c r="AG18" s="21">
         <v>10</v>
       </c>
       <c r="AH18" s="3">
@@ -3375,25 +3570,25 @@
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C19" s="17">
+        <v>103</v>
+      </c>
+      <c r="C19" s="23">
         <v>18</v>
       </c>
-      <c r="D19" s="17">
-        <v>1</v>
-      </c>
-      <c r="E19" s="19">
+      <c r="D19" s="23">
+        <v>1</v>
+      </c>
+      <c r="E19" s="25">
         <v>0.7</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="25">
         <v>0</v>
       </c>
       <c r="H19" s="7">
@@ -3462,7 +3657,7 @@
       <c r="AC19" s="4">
         <v>0</v>
       </c>
-      <c r="AD19" s="15">
+      <c r="AD19" s="21">
         <v>18</v>
       </c>
       <c r="AE19" s="3">
@@ -3492,25 +3687,25 @@
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="17">
+        <v>104</v>
+      </c>
+      <c r="C20" s="23">
         <v>19</v>
       </c>
-      <c r="D20" s="17">
-        <v>1</v>
-      </c>
-      <c r="E20" s="19">
+      <c r="D20" s="23">
+        <v>1</v>
+      </c>
+      <c r="E20" s="25">
         <v>0.7</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="25">
         <v>0</v>
       </c>
       <c r="H20" s="7">
@@ -3547,7 +3742,7 @@
         <v>3</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="T20" s="2" t="s">
         <v>27</v>
@@ -3556,7 +3751,7 @@
         <v>6</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="W20" s="1">
         <v>0</v>
@@ -3574,12 +3769,12 @@
         <v>14.5</v>
       </c>
       <c r="AB20" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AC20" s="4">
         <v>0</v>
       </c>
-      <c r="AD20" s="15">
+      <c r="AD20" s="21">
         <v>18</v>
       </c>
       <c r="AE20" s="3">
@@ -3609,55 +3804,55 @@
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="17">
+        <v>107</v>
+      </c>
+      <c r="C21" s="23">
         <v>20</v>
       </c>
-      <c r="D21" s="17">
-        <v>1</v>
-      </c>
-      <c r="E21" s="19">
-        <v>1</v>
-      </c>
-      <c r="F21" s="20">
+      <c r="D21" s="23">
+        <v>1</v>
+      </c>
+      <c r="E21" s="25">
+        <v>1</v>
+      </c>
+      <c r="F21" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="25">
         <v>-0.33</v>
       </c>
-      <c r="H21" s="17">
-        <v>0</v>
-      </c>
-      <c r="I21" s="17">
-        <v>0</v>
-      </c>
-      <c r="J21" s="17">
-        <v>0</v>
-      </c>
-      <c r="K21" s="17">
-        <v>0</v>
-      </c>
-      <c r="L21" s="17">
-        <v>0</v>
-      </c>
-      <c r="M21" s="17">
-        <v>0</v>
-      </c>
-      <c r="N21" s="17">
-        <v>1</v>
-      </c>
-      <c r="O21" s="17">
-        <v>0</v>
-      </c>
-      <c r="P21" s="22">
+      <c r="H21" s="23">
+        <v>0</v>
+      </c>
+      <c r="I21" s="23">
+        <v>0</v>
+      </c>
+      <c r="J21" s="23">
+        <v>0</v>
+      </c>
+      <c r="K21" s="23">
+        <v>0</v>
+      </c>
+      <c r="L21" s="23">
+        <v>0</v>
+      </c>
+      <c r="M21" s="23">
+        <v>0</v>
+      </c>
+      <c r="N21" s="23">
+        <v>1</v>
+      </c>
+      <c r="O21" s="23">
+        <v>0</v>
+      </c>
+      <c r="P21" s="28">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="Q21" s="17">
+      <c r="Q21" s="23">
         <v>30</v>
       </c>
       <c r="R21" s="4">
@@ -3682,7 +3877,7 @@
         <v>17</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Z21" s="1">
         <v>0</v>
@@ -3696,7 +3891,7 @@
       <c r="AC21" s="4">
         <v>0</v>
       </c>
-      <c r="AD21" s="15">
+      <c r="AD21" s="21">
         <v>30</v>
       </c>
       <c r="AE21" s="3">
@@ -3726,55 +3921,55 @@
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="17">
+        <v>108</v>
+      </c>
+      <c r="C22" s="23">
         <v>21</v>
       </c>
-      <c r="D22" s="17">
-        <v>1</v>
-      </c>
-      <c r="E22" s="19">
-        <v>1</v>
-      </c>
-      <c r="F22" s="20">
+      <c r="D22" s="23">
+        <v>1</v>
+      </c>
+      <c r="E22" s="25">
+        <v>1</v>
+      </c>
+      <c r="F22" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="25">
         <v>0.33</v>
       </c>
-      <c r="H22" s="17">
-        <v>0</v>
-      </c>
-      <c r="I22" s="17">
-        <v>0</v>
-      </c>
-      <c r="J22" s="17">
-        <v>0</v>
-      </c>
-      <c r="K22" s="17">
-        <v>0</v>
-      </c>
-      <c r="L22" s="17">
-        <v>0</v>
-      </c>
-      <c r="M22" s="17">
-        <v>0</v>
-      </c>
-      <c r="N22" s="17">
-        <v>1</v>
-      </c>
-      <c r="O22" s="17">
-        <v>0</v>
-      </c>
-      <c r="P22" s="22">
+      <c r="H22" s="23">
+        <v>0</v>
+      </c>
+      <c r="I22" s="23">
+        <v>0</v>
+      </c>
+      <c r="J22" s="23">
+        <v>0</v>
+      </c>
+      <c r="K22" s="23">
+        <v>0</v>
+      </c>
+      <c r="L22" s="23">
+        <v>0</v>
+      </c>
+      <c r="M22" s="23">
+        <v>0</v>
+      </c>
+      <c r="N22" s="23">
+        <v>1</v>
+      </c>
+      <c r="O22" s="23">
+        <v>0</v>
+      </c>
+      <c r="P22" s="28">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="Q22" s="17">
+      <c r="Q22" s="23">
         <v>30</v>
       </c>
       <c r="R22" s="4">
@@ -3813,7 +4008,7 @@
       <c r="AC22" s="4">
         <v>0</v>
       </c>
-      <c r="AD22" s="15">
+      <c r="AD22" s="21">
         <v>30</v>
       </c>
       <c r="AE22" s="3">
@@ -3846,58 +4041,58 @@
         <v>40</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23" s="17">
+        <v>101</v>
+      </c>
+      <c r="C23" s="23">
         <v>22</v>
       </c>
-      <c r="D23" s="17">
-        <v>1</v>
-      </c>
-      <c r="E23" s="19">
-        <v>1</v>
-      </c>
-      <c r="F23" s="23">
+      <c r="D23" s="23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="25">
+        <v>1</v>
+      </c>
+      <c r="F23" s="29">
         <f>Input!H2</f>
         <v>1</v>
       </c>
-      <c r="G23" s="19">
-        <v>1</v>
-      </c>
-      <c r="H23" s="17">
-        <v>0</v>
-      </c>
-      <c r="I23" s="17">
-        <v>0</v>
-      </c>
-      <c r="J23" s="17">
-        <v>0</v>
-      </c>
-      <c r="K23" s="17">
-        <v>0</v>
-      </c>
-      <c r="L23" s="17">
-        <v>0</v>
-      </c>
-      <c r="M23" s="17">
-        <v>0</v>
-      </c>
-      <c r="N23" s="17">
-        <v>1</v>
-      </c>
-      <c r="O23" s="17">
-        <v>0</v>
-      </c>
-      <c r="P23" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="17">
+      <c r="G23" s="25">
+        <v>1</v>
+      </c>
+      <c r="H23" s="23">
+        <v>0</v>
+      </c>
+      <c r="I23" s="23">
+        <v>0</v>
+      </c>
+      <c r="J23" s="23">
+        <v>0</v>
+      </c>
+      <c r="K23" s="23">
+        <v>0</v>
+      </c>
+      <c r="L23" s="23">
+        <v>0</v>
+      </c>
+      <c r="M23" s="23">
+        <v>0</v>
+      </c>
+      <c r="N23" s="23">
+        <v>1</v>
+      </c>
+      <c r="O23" s="23">
+        <v>0</v>
+      </c>
+      <c r="P23" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="23">
         <v>52</v>
       </c>
       <c r="R23" s="4">
         <v>3</v>
       </c>
-      <c r="S23" s="28">
+      <c r="S23" s="34">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) + 0.025</f>
         <v>1.0316739272428239</v>
       </c>
@@ -3907,7 +4102,7 @@
       <c r="U23" s="1">
         <v>10</v>
       </c>
-      <c r="V23" s="28">
+      <c r="V23" s="34">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) - 0.025</f>
         <v>0.98167392724282398</v>
       </c>
@@ -3917,7 +4112,7 @@
       <c r="X23" s="1">
         <v>17</v>
       </c>
-      <c r="Y23" s="28">
+      <c r="Y23" s="34">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2)</f>
         <v>1.006673927242824</v>
       </c>
@@ -3927,7 +4122,7 @@
       <c r="AA23" s="1">
         <v>24</v>
       </c>
-      <c r="AB23" s="28">
+      <c r="AB23" s="34">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) + 0.05</f>
         <v>1.0566739272428241</v>
       </c>
@@ -3937,7 +4132,7 @@
       <c r="AD23" s="4">
         <v>31</v>
       </c>
-      <c r="AE23" s="28">
+      <c r="AE23" s="34">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2)</f>
         <v>1.006673927242824</v>
       </c>
@@ -3947,7 +4142,7 @@
       <c r="AG23" s="1">
         <v>38</v>
       </c>
-      <c r="AH23" s="28">
+      <c r="AH23" s="34">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) - 0.05</f>
         <v>0.95667392724282396</v>
       </c>
@@ -3957,7 +4152,7 @@
       <c r="AJ23" s="1">
         <v>45</v>
       </c>
-      <c r="AK23" s="28">
+      <c r="AK23" s="34">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2)</f>
         <v>1.006673927242824</v>
       </c>
@@ -3967,25 +4162,25 @@
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="17">
+        <v>98</v>
+      </c>
+      <c r="C24" s="23">
         <v>23</v>
       </c>
-      <c r="D24" s="17">
-        <v>1</v>
-      </c>
-      <c r="E24" s="19">
+      <c r="D24" s="23">
+        <v>1</v>
+      </c>
+      <c r="E24" s="25">
         <v>0.7</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F24" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="25">
         <v>0</v>
       </c>
       <c r="H24" s="7">
@@ -4015,7 +4210,7 @@
       <c r="P24" s="7">
         <v>1</v>
       </c>
-      <c r="Q24" s="8">
+      <c r="Q24" s="12">
         <v>80</v>
       </c>
       <c r="R24" s="4">
@@ -4027,7 +4222,7 @@
       <c r="T24" s="1">
         <v>0</v>
       </c>
-      <c r="U24" s="14">
+      <c r="U24" s="20">
         <v>80</v>
       </c>
       <c r="V24" s="3">
@@ -4084,25 +4279,25 @@
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="17">
+        <v>95</v>
+      </c>
+      <c r="C25" s="23">
         <v>24</v>
       </c>
-      <c r="D25" s="17">
-        <v>1</v>
-      </c>
-      <c r="E25" s="19">
+      <c r="D25" s="23">
+        <v>1</v>
+      </c>
+      <c r="E25" s="25">
         <v>0.5</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="25">
         <v>0</v>
       </c>
       <c r="H25" s="7">
@@ -4132,7 +4327,7 @@
       <c r="P25" s="7">
         <v>1</v>
       </c>
-      <c r="Q25" s="8">
+      <c r="Q25" s="12">
         <v>80</v>
       </c>
       <c r="R25" s="4">
@@ -4144,7 +4339,7 @@
       <c r="T25" s="1">
         <v>0</v>
       </c>
-      <c r="U25" s="14">
+      <c r="U25" s="20">
         <v>80</v>
       </c>
       <c r="V25" s="3">
@@ -4198,7 +4393,7 @@
       <c r="AL25" s="3">
         <v>0</v>
       </c>
-      <c r="AQ25" s="28">
+      <c r="AQ25" s="34">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) + 0.025</f>
         <v>1.0316739272428239</v>
       </c>
@@ -4208,52 +4403,52 @@
         <v>35</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C26" s="17">
+        <v>105</v>
+      </c>
+      <c r="C26" s="23">
         <v>25</v>
       </c>
-      <c r="D26" s="17">
-        <v>1</v>
-      </c>
-      <c r="E26" s="19">
+      <c r="D26" s="23">
+        <v>1</v>
+      </c>
+      <c r="E26" s="25">
         <v>0.7</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G26" s="19">
-        <v>0</v>
-      </c>
-      <c r="H26" s="17">
-        <v>0</v>
-      </c>
-      <c r="I26" s="17">
-        <v>0</v>
-      </c>
-      <c r="J26" s="17">
-        <v>0</v>
-      </c>
-      <c r="K26" s="17">
-        <v>0</v>
-      </c>
-      <c r="L26" s="17">
-        <v>0</v>
-      </c>
-      <c r="M26" s="17">
-        <v>0</v>
-      </c>
-      <c r="N26" s="17">
-        <v>0</v>
-      </c>
-      <c r="O26" s="17">
-        <v>1</v>
-      </c>
-      <c r="P26" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="17">
+      <c r="G26" s="25">
+        <v>0</v>
+      </c>
+      <c r="H26" s="23">
+        <v>0</v>
+      </c>
+      <c r="I26" s="23">
+        <v>0</v>
+      </c>
+      <c r="J26" s="23">
+        <v>0</v>
+      </c>
+      <c r="K26" s="23">
+        <v>0</v>
+      </c>
+      <c r="L26" s="23">
+        <v>0</v>
+      </c>
+      <c r="M26" s="23">
+        <v>0</v>
+      </c>
+      <c r="N26" s="23">
+        <v>0</v>
+      </c>
+      <c r="O26" s="23">
+        <v>1</v>
+      </c>
+      <c r="P26" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="23">
         <v>80</v>
       </c>
       <c r="R26" s="4">
@@ -4278,7 +4473,7 @@
         <v>42</v>
       </c>
       <c r="Y26" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z26" s="1">
         <v>0</v>
@@ -4292,7 +4487,7 @@
       <c r="AC26" s="4">
         <v>0</v>
       </c>
-      <c r="AD26" s="15">
+      <c r="AD26" s="21">
         <v>80</v>
       </c>
       <c r="AE26" s="3">
@@ -4325,52 +4520,52 @@
         <v>39</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" s="17">
+        <v>106</v>
+      </c>
+      <c r="C27" s="23">
         <v>26</v>
       </c>
-      <c r="D27" s="17">
-        <v>1</v>
-      </c>
-      <c r="E27" s="19">
+      <c r="D27" s="23">
+        <v>1</v>
+      </c>
+      <c r="E27" s="25">
         <v>0.7</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G27" s="19">
-        <v>0</v>
-      </c>
-      <c r="H27" s="17">
-        <v>0</v>
-      </c>
-      <c r="I27" s="17">
-        <v>0</v>
-      </c>
-      <c r="J27" s="17">
-        <v>0</v>
-      </c>
-      <c r="K27" s="17">
-        <v>0</v>
-      </c>
-      <c r="L27" s="17">
-        <v>0</v>
-      </c>
-      <c r="M27" s="17">
-        <v>0</v>
-      </c>
-      <c r="N27" s="17">
-        <v>0</v>
-      </c>
-      <c r="O27" s="17">
-        <v>1</v>
-      </c>
-      <c r="P27" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="17">
+      <c r="G27" s="25">
+        <v>0</v>
+      </c>
+      <c r="H27" s="23">
+        <v>0</v>
+      </c>
+      <c r="I27" s="23">
+        <v>0</v>
+      </c>
+      <c r="J27" s="23">
+        <v>0</v>
+      </c>
+      <c r="K27" s="23">
+        <v>0</v>
+      </c>
+      <c r="L27" s="23">
+        <v>0</v>
+      </c>
+      <c r="M27" s="23">
+        <v>0</v>
+      </c>
+      <c r="N27" s="23">
+        <v>0</v>
+      </c>
+      <c r="O27" s="23">
+        <v>1</v>
+      </c>
+      <c r="P27" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="23">
         <v>80</v>
       </c>
       <c r="R27" s="4">
@@ -4395,7 +4590,7 @@
         <v>42</v>
       </c>
       <c r="Y27" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Z27" s="1">
         <v>0</v>
@@ -4409,7 +4604,7 @@
       <c r="AC27" s="4">
         <v>0</v>
       </c>
-      <c r="AD27" s="15">
+      <c r="AD27" s="21">
         <v>80</v>
       </c>
       <c r="AE27" s="3">
@@ -4439,25 +4634,25 @@
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="17">
+        <v>97</v>
+      </c>
+      <c r="C28" s="23">
         <v>27</v>
       </c>
-      <c r="D28" s="17">
-        <v>1</v>
-      </c>
-      <c r="E28" s="19">
-        <v>1</v>
-      </c>
-      <c r="F28" s="20">
+      <c r="D28" s="23">
+        <v>1</v>
+      </c>
+      <c r="E28" s="25">
+        <v>1</v>
+      </c>
+      <c r="F28" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="25">
         <v>0</v>
       </c>
       <c r="H28" s="7">
@@ -4487,7 +4682,7 @@
       <c r="P28" s="7">
         <v>1</v>
       </c>
-      <c r="Q28" s="8">
+      <c r="Q28" s="12">
         <v>100</v>
       </c>
       <c r="R28" s="4">
@@ -4499,7 +4694,7 @@
       <c r="T28" s="1">
         <v>0</v>
       </c>
-      <c r="U28" s="14">
+      <c r="U28" s="20">
         <v>100</v>
       </c>
       <c r="V28" s="3">
@@ -4556,25 +4751,25 @@
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="17">
+        <v>96</v>
+      </c>
+      <c r="C29" s="23">
         <v>28</v>
       </c>
-      <c r="D29" s="17">
-        <v>1</v>
-      </c>
-      <c r="E29" s="19">
+      <c r="D29" s="23">
+        <v>1</v>
+      </c>
+      <c r="E29" s="25">
         <v>0.7</v>
       </c>
-      <c r="F29" s="20">
+      <c r="F29" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G29" s="19">
+      <c r="G29" s="25">
         <v>0</v>
       </c>
       <c r="H29" s="7">
@@ -4604,7 +4799,7 @@
       <c r="P29" s="7">
         <v>1</v>
       </c>
-      <c r="Q29" s="8">
+      <c r="Q29" s="12">
         <v>100</v>
       </c>
       <c r="R29" s="4">
@@ -4616,7 +4811,7 @@
       <c r="T29" s="1">
         <v>0</v>
       </c>
-      <c r="U29" s="14">
+      <c r="U29" s="20">
         <v>100</v>
       </c>
       <c r="V29" s="3">
@@ -4676,22 +4871,22 @@
         <v>41</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="17">
+        <v>102</v>
+      </c>
+      <c r="C30" s="23">
         <v>29</v>
       </c>
-      <c r="D30" s="17">
-        <v>1</v>
-      </c>
-      <c r="E30" s="19">
+      <c r="D30" s="23">
+        <v>1</v>
+      </c>
+      <c r="E30" s="25">
         <v>0.3</v>
       </c>
-      <c r="F30" s="23">
+      <c r="F30" s="29">
         <f>Input!I2</f>
         <v>2</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="25">
         <v>0.99</v>
       </c>
       <c r="H30" s="7">
@@ -4760,7 +4955,7 @@
       <c r="AC30" s="1">
         <v>0</v>
       </c>
-      <c r="AD30" s="15">
+      <c r="AD30" s="21">
         <v>140</v>
       </c>
       <c r="AE30" s="3">
@@ -4793,22 +4988,22 @@
         <v>38</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="17">
+        <v>100</v>
+      </c>
+      <c r="C31" s="23">
         <v>30</v>
       </c>
-      <c r="D31" s="17">
-        <v>1</v>
-      </c>
-      <c r="E31" s="19">
-        <v>1</v>
-      </c>
-      <c r="F31" s="20">
+      <c r="D31" s="23">
+        <v>1</v>
+      </c>
+      <c r="E31" s="25">
+        <v>1</v>
+      </c>
+      <c r="F31" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G31" s="19">
+      <c r="G31" s="25">
         <v>0</v>
       </c>
       <c r="H31" s="7">
@@ -4877,7 +5072,7 @@
       <c r="AC31" s="1">
         <v>0</v>
       </c>
-      <c r="AD31" s="15">
+      <c r="AD31" s="21">
         <v>145</v>
       </c>
       <c r="AE31" s="3">
@@ -4910,22 +5105,22 @@
         <v>38</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="17">
+        <v>99</v>
+      </c>
+      <c r="C32" s="23">
         <v>31</v>
       </c>
-      <c r="D32" s="17">
-        <v>1</v>
-      </c>
-      <c r="E32" s="19">
-        <v>1</v>
-      </c>
-      <c r="F32" s="20">
+      <c r="D32" s="23">
+        <v>1</v>
+      </c>
+      <c r="E32" s="25">
+        <v>1</v>
+      </c>
+      <c r="F32" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G32" s="19">
+      <c r="G32" s="25">
         <v>0</v>
       </c>
       <c r="H32" s="7">
@@ -4994,7 +5189,7 @@
       <c r="AC32" s="1">
         <v>0</v>
       </c>
-      <c r="AD32" s="15">
+      <c r="AD32" s="21">
         <v>145</v>
       </c>
       <c r="AE32" s="3">
@@ -5024,25 +5219,25 @@
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="17">
+        <v>94</v>
+      </c>
+      <c r="C33" s="23">
         <v>32</v>
       </c>
-      <c r="D33" s="17">
-        <v>1</v>
-      </c>
-      <c r="E33" s="19">
-        <v>0</v>
-      </c>
-      <c r="F33" s="20">
+      <c r="D33" s="23">
+        <v>1</v>
+      </c>
+      <c r="E33" s="25">
+        <v>0</v>
+      </c>
+      <c r="F33" s="26">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G33" s="19">
+      <c r="G33" s="25">
         <v>0</v>
       </c>
       <c r="H33" s="7">
@@ -5084,7 +5279,7 @@
       <c r="T33" s="1">
         <v>0</v>
       </c>
-      <c r="U33" s="15">
+      <c r="U33" s="21">
         <v>155</v>
       </c>
       <c r="V33" s="3">
@@ -5156,91 +5351,300 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E2 E4 E6 E8 E10 E12 E14 E16">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3 E5 E7 E9 E11 E13 E15 E17">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="16">
+        <v>2</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="9">
+        <v>3</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="9">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="9">
+        <v>5</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
+        <v>6</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="9">
+        <v>7</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="9">
+        <v>-0.33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="9">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="9">
+        <v>10</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="9">
+        <v>-0.33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="9">
+        <v>11</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="9">
+        <v>12</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="9">
+        <v>-0.33</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:C13">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -5248,4 +5652,143 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="5" width="48.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>140</v>
+      </c>
+      <c r="E19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
"Balance" tab removed, example alligned
</commit_message>
<xml_diff>
--- a/PSCAD/DK1_DSO_D/TestCases.xlsx
+++ b/PSCAD/DK1_DSO_D/TestCases.xlsx
@@ -5,17 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MKT.ENERGINET\Desktop\PP-MTB-Alpha\PP-MTB PSCAD\DK1_DSO_D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\energinet.local\endk_funktion\Projekter\EffektGruppen\13_Medarbejdermapper\CVL\PP-MTB\PSCAD\DK1_DSO_D\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="350"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="2" r:id="rId1"/>
     <sheet name="Cases" sheetId="1" r:id="rId2"/>
-    <sheet name="Balance" sheetId="3" r:id="rId3"/>
-    <sheet name="PSCAD Compliers" sheetId="4" r:id="rId4"/>
+    <sheet name="PSCAD Compliers" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Input!$A$1:$M$2</definedName>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="144">
   <si>
     <t>PrefCtrl</t>
   </si>
@@ -171,9 +170,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>Balance</t>
-  </si>
-  <si>
     <t>P0</t>
   </si>
   <si>
@@ -264,23 +260,10 @@
     <t>Qmode_PF: Power factor control</t>
   </si>
   <si>
-    <t>Additional information:
-An overview of all the balances tested</t>
-  </si>
-  <si>
     <t>Qmode</t>
   </si>
   <si>
     <t>InitValue</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>PF</t>
-  </si>
-  <si>
-    <t>V</t>
   </si>
   <si>
     <t>TestType</t>
@@ -569,7 +552,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,13 +562,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -683,7 +659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -706,22 +682,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -730,16 +694,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -757,7 +715,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -769,13 +727,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -792,17 +750,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1261,18 +1209,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="15" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="8" style="15" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="15"/>
+    <col min="2" max="2" width="6.42578125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="8" style="11" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="11"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
@@ -1282,64 +1228,64 @@
     <col min="13" max="13" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="14" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="C1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="D1" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="E1" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>145</v>
+      <c r="J1" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="15">
+      <c r="B2" s="11">
         <v>10</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="11">
         <v>10</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="11">
         <v>62.5</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="11">
         <v>5</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="11">
         <v>15</v>
       </c>
       <c r="G2">
@@ -1352,10 +1298,10 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="K2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L2">
         <v>2</v>
@@ -1368,36 +1314,36 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G4" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="K4" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="N4" s="32" t="s">
-        <v>146</v>
+      <c r="G4" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G6" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G6" s="32" t="s">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G7" s="26" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G7" s="32" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G8" s="26" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G8" s="32" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1468,67 +1414,67 @@
         <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="23" t="s">
+      <c r="D1" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q1" s="24" t="s">
+      <c r="P1" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q1" s="18" t="s">
         <v>8</v>
       </c>
       <c r="R1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="8" t="s">
         <v>15</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>16</v>
@@ -1537,7 +1483,7 @@
         <v>17</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Z1" s="4" t="s">
         <v>18</v>
@@ -1546,7 +1492,7 @@
         <v>19</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>20</v>
@@ -1555,7 +1501,7 @@
         <v>21</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>22</v>
@@ -1564,72 +1510,72 @@
         <v>30</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>31</v>
       </c>
       <c r="AJ1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="23">
-        <v>1</v>
-      </c>
-      <c r="D2" s="23">
-        <v>1</v>
-      </c>
-      <c r="E2" s="25">
-        <v>1</v>
-      </c>
-      <c r="F2" s="26">
+        <v>76</v>
+      </c>
+      <c r="C2" s="17">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17">
+        <v>1</v>
+      </c>
+      <c r="E2" s="19">
+        <v>1</v>
+      </c>
+      <c r="F2" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G2" s="25">
-        <v>0</v>
-      </c>
-      <c r="H2" s="23">
-        <v>0</v>
-      </c>
-      <c r="I2" s="23">
-        <v>0</v>
-      </c>
-      <c r="J2" s="23">
+      <c r="G2" s="19">
+        <v>0</v>
+      </c>
+      <c r="H2" s="17">
+        <v>0</v>
+      </c>
+      <c r="I2" s="17">
+        <v>0</v>
+      </c>
+      <c r="J2" s="17">
         <v>7</v>
       </c>
       <c r="K2" s="7">
         <v>0.01</v>
       </c>
-      <c r="L2" s="27">
+      <c r="L2" s="21">
         <v>0.15</v>
       </c>
-      <c r="M2" s="23">
-        <v>0</v>
-      </c>
-      <c r="N2" s="23">
-        <v>0</v>
-      </c>
-      <c r="O2" s="23">
-        <v>0</v>
-      </c>
-      <c r="P2" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="23">
+      <c r="M2" s="17">
+        <v>0</v>
+      </c>
+      <c r="N2" s="17">
+        <v>0</v>
+      </c>
+      <c r="O2" s="17">
+        <v>0</v>
+      </c>
+      <c r="P2" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="17">
         <v>4</v>
       </c>
       <c r="R2" s="4">
@@ -1641,7 +1587,7 @@
       <c r="T2" s="4">
         <v>0</v>
       </c>
-      <c r="U2" s="21">
+      <c r="U2" s="15">
         <v>4</v>
       </c>
       <c r="V2" s="3">
@@ -1698,55 +1644,55 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="23">
+        <v>77</v>
+      </c>
+      <c r="C3" s="17">
         <v>2</v>
       </c>
-      <c r="D3" s="23">
-        <v>1</v>
-      </c>
-      <c r="E3" s="25">
-        <v>1</v>
-      </c>
-      <c r="F3" s="26">
+      <c r="D3" s="17">
+        <v>1</v>
+      </c>
+      <c r="E3" s="19">
+        <v>1</v>
+      </c>
+      <c r="F3" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G3" s="25">
-        <v>0</v>
-      </c>
-      <c r="H3" s="23">
-        <v>0</v>
-      </c>
-      <c r="I3" s="23">
-        <v>0</v>
-      </c>
-      <c r="J3" s="23">
+      <c r="G3" s="19">
+        <v>0</v>
+      </c>
+      <c r="H3" s="17">
+        <v>0</v>
+      </c>
+      <c r="I3" s="17">
+        <v>0</v>
+      </c>
+      <c r="J3" s="17">
         <v>7</v>
       </c>
-      <c r="K3" s="27">
+      <c r="K3" s="21">
         <v>0.2</v>
       </c>
-      <c r="L3" s="27">
+      <c r="L3" s="21">
         <v>0.45</v>
       </c>
-      <c r="M3" s="23">
-        <v>0</v>
-      </c>
-      <c r="N3" s="23">
-        <v>0</v>
-      </c>
-      <c r="O3" s="23">
-        <v>0</v>
-      </c>
-      <c r="P3" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="23">
+      <c r="M3" s="17">
+        <v>0</v>
+      </c>
+      <c r="N3" s="17">
+        <v>0</v>
+      </c>
+      <c r="O3" s="17">
+        <v>0</v>
+      </c>
+      <c r="P3" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="17">
         <v>4</v>
       </c>
       <c r="R3" s="4">
@@ -1758,7 +1704,7 @@
       <c r="T3" s="4">
         <v>0</v>
       </c>
-      <c r="U3" s="21">
+      <c r="U3" s="15">
         <v>4</v>
       </c>
       <c r="V3" s="3">
@@ -1815,55 +1761,55 @@
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="23">
+        <v>78</v>
+      </c>
+      <c r="C4" s="17">
         <v>3</v>
       </c>
-      <c r="D4" s="23">
-        <v>1</v>
-      </c>
-      <c r="E4" s="25">
-        <v>1</v>
-      </c>
-      <c r="F4" s="26">
+      <c r="D4" s="17">
+        <v>1</v>
+      </c>
+      <c r="E4" s="19">
+        <v>1</v>
+      </c>
+      <c r="F4" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G4" s="25">
-        <v>0</v>
-      </c>
-      <c r="H4" s="23">
-        <v>0</v>
-      </c>
-      <c r="I4" s="23">
-        <v>0</v>
-      </c>
-      <c r="J4" s="23">
+      <c r="G4" s="19">
+        <v>0</v>
+      </c>
+      <c r="H4" s="17">
+        <v>0</v>
+      </c>
+      <c r="I4" s="17">
+        <v>0</v>
+      </c>
+      <c r="J4" s="17">
         <v>4</v>
       </c>
-      <c r="K4" s="28">
+      <c r="K4" s="22">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="L4" s="27">
+      <c r="L4" s="21">
         <v>0.15</v>
       </c>
-      <c r="M4" s="23">
-        <v>0</v>
-      </c>
-      <c r="N4" s="23">
-        <v>0</v>
-      </c>
-      <c r="O4" s="23">
-        <v>0</v>
-      </c>
-      <c r="P4" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="23">
+      <c r="M4" s="17">
+        <v>0</v>
+      </c>
+      <c r="N4" s="17">
+        <v>0</v>
+      </c>
+      <c r="O4" s="17">
+        <v>0</v>
+      </c>
+      <c r="P4" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="17">
         <v>4</v>
       </c>
       <c r="R4" s="4">
@@ -1875,7 +1821,7 @@
       <c r="T4" s="4">
         <v>0</v>
       </c>
-      <c r="U4" s="21">
+      <c r="U4" s="15">
         <v>4</v>
       </c>
       <c r="V4" s="3">
@@ -1932,55 +1878,55 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="23">
+        <v>79</v>
+      </c>
+      <c r="C5" s="17">
         <v>4</v>
       </c>
-      <c r="D5" s="23">
-        <v>1</v>
-      </c>
-      <c r="E5" s="25">
-        <v>1</v>
-      </c>
-      <c r="F5" s="26">
+      <c r="D5" s="17">
+        <v>1</v>
+      </c>
+      <c r="E5" s="19">
+        <v>1</v>
+      </c>
+      <c r="F5" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G5" s="25">
-        <v>0</v>
-      </c>
-      <c r="H5" s="23">
-        <v>0</v>
-      </c>
-      <c r="I5" s="23">
-        <v>0</v>
-      </c>
-      <c r="J5" s="23">
+      <c r="G5" s="19">
+        <v>0</v>
+      </c>
+      <c r="H5" s="17">
+        <v>0</v>
+      </c>
+      <c r="I5" s="17">
+        <v>0</v>
+      </c>
+      <c r="J5" s="17">
         <v>4</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K5" s="21">
         <v>0.2</v>
       </c>
-      <c r="L5" s="27">
+      <c r="L5" s="21">
         <v>0.45</v>
       </c>
-      <c r="M5" s="23">
-        <v>0</v>
-      </c>
-      <c r="N5" s="23">
-        <v>0</v>
-      </c>
-      <c r="O5" s="23">
-        <v>0</v>
-      </c>
-      <c r="P5" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="23">
+      <c r="M5" s="17">
+        <v>0</v>
+      </c>
+      <c r="N5" s="17">
+        <v>0</v>
+      </c>
+      <c r="O5" s="17">
+        <v>0</v>
+      </c>
+      <c r="P5" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="17">
         <v>4</v>
       </c>
       <c r="R5" s="4">
@@ -1992,7 +1938,7 @@
       <c r="T5" s="4">
         <v>0</v>
       </c>
-      <c r="U5" s="21">
+      <c r="U5" s="15">
         <v>4</v>
       </c>
       <c r="V5" s="3">
@@ -2049,55 +1995,55 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="23">
+        <v>80</v>
+      </c>
+      <c r="C6" s="17">
         <v>5</v>
       </c>
-      <c r="D6" s="23">
-        <v>1</v>
-      </c>
-      <c r="E6" s="25">
-        <v>1</v>
-      </c>
-      <c r="F6" s="26">
+      <c r="D6" s="17">
+        <v>1</v>
+      </c>
+      <c r="E6" s="19">
+        <v>1</v>
+      </c>
+      <c r="F6" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G6" s="25">
-        <v>0</v>
-      </c>
-      <c r="H6" s="23">
-        <v>0</v>
-      </c>
-      <c r="I6" s="23">
-        <v>0</v>
-      </c>
-      <c r="J6" s="23">
-        <v>1</v>
-      </c>
-      <c r="K6" s="28">
+      <c r="G6" s="19">
+        <v>0</v>
+      </c>
+      <c r="H6" s="17">
+        <v>0</v>
+      </c>
+      <c r="I6" s="17">
+        <v>0</v>
+      </c>
+      <c r="J6" s="17">
+        <v>1</v>
+      </c>
+      <c r="K6" s="22">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="L6" s="27">
+      <c r="L6" s="21">
         <v>0.15</v>
       </c>
-      <c r="M6" s="23">
-        <v>0</v>
-      </c>
-      <c r="N6" s="23">
-        <v>0</v>
-      </c>
-      <c r="O6" s="23">
-        <v>0</v>
-      </c>
-      <c r="P6" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="23">
+      <c r="M6" s="17">
+        <v>0</v>
+      </c>
+      <c r="N6" s="17">
+        <v>0</v>
+      </c>
+      <c r="O6" s="17">
+        <v>0</v>
+      </c>
+      <c r="P6" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="17">
         <v>4</v>
       </c>
       <c r="R6" s="4">
@@ -2109,7 +2055,7 @@
       <c r="T6" s="4">
         <v>0</v>
       </c>
-      <c r="U6" s="21">
+      <c r="U6" s="15">
         <v>4</v>
       </c>
       <c r="V6" s="3">
@@ -2166,55 +2112,55 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="23">
+        <v>81</v>
+      </c>
+      <c r="C7" s="17">
         <v>6</v>
       </c>
-      <c r="D7" s="23">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25">
-        <v>1</v>
-      </c>
-      <c r="F7" s="26">
+      <c r="D7" s="17">
+        <v>1</v>
+      </c>
+      <c r="E7" s="19">
+        <v>1</v>
+      </c>
+      <c r="F7" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G7" s="25">
-        <v>0</v>
-      </c>
-      <c r="H7" s="23">
-        <v>0</v>
-      </c>
-      <c r="I7" s="23">
-        <v>0</v>
-      </c>
-      <c r="J7" s="23">
-        <v>1</v>
-      </c>
-      <c r="K7" s="27">
+      <c r="G7" s="19">
+        <v>0</v>
+      </c>
+      <c r="H7" s="17">
+        <v>0</v>
+      </c>
+      <c r="I7" s="17">
+        <v>0</v>
+      </c>
+      <c r="J7" s="17">
+        <v>1</v>
+      </c>
+      <c r="K7" s="21">
         <v>0.2</v>
       </c>
-      <c r="L7" s="27">
+      <c r="L7" s="21">
         <v>0.45</v>
       </c>
-      <c r="M7" s="23">
-        <v>0</v>
-      </c>
-      <c r="N7" s="23">
-        <v>0</v>
-      </c>
-      <c r="O7" s="23">
-        <v>0</v>
-      </c>
-      <c r="P7" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="23">
+      <c r="M7" s="17">
+        <v>0</v>
+      </c>
+      <c r="N7" s="17">
+        <v>0</v>
+      </c>
+      <c r="O7" s="17">
+        <v>0</v>
+      </c>
+      <c r="P7" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="17">
         <v>4</v>
       </c>
       <c r="R7" s="4">
@@ -2226,7 +2172,7 @@
       <c r="T7" s="4">
         <v>0</v>
       </c>
-      <c r="U7" s="21">
+      <c r="U7" s="15">
         <v>4</v>
       </c>
       <c r="V7" s="3">
@@ -2283,55 +2229,55 @@
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="23">
+        <v>82</v>
+      </c>
+      <c r="C8" s="17">
         <v>7</v>
       </c>
-      <c r="D8" s="23">
-        <v>1</v>
-      </c>
-      <c r="E8" s="25">
-        <v>1</v>
-      </c>
-      <c r="F8" s="26">
+      <c r="D8" s="17">
+        <v>1</v>
+      </c>
+      <c r="E8" s="19">
+        <v>1</v>
+      </c>
+      <c r="F8" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G8" s="25">
-        <v>0</v>
-      </c>
-      <c r="H8" s="23">
-        <v>0</v>
-      </c>
-      <c r="I8" s="23">
-        <v>0</v>
-      </c>
-      <c r="J8" s="23">
+      <c r="G8" s="19">
+        <v>0</v>
+      </c>
+      <c r="H8" s="17">
+        <v>0</v>
+      </c>
+      <c r="I8" s="17">
+        <v>0</v>
+      </c>
+      <c r="J8" s="17">
         <v>7</v>
       </c>
-      <c r="K8" s="27">
+      <c r="K8" s="21">
         <v>0.4</v>
       </c>
-      <c r="L8" s="27">
+      <c r="L8" s="21">
         <v>0.75</v>
       </c>
-      <c r="M8" s="23">
-        <v>0</v>
-      </c>
-      <c r="N8" s="23">
-        <v>0</v>
-      </c>
-      <c r="O8" s="23">
-        <v>0</v>
-      </c>
-      <c r="P8" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="23">
+      <c r="M8" s="17">
+        <v>0</v>
+      </c>
+      <c r="N8" s="17">
+        <v>0</v>
+      </c>
+      <c r="O8" s="17">
+        <v>0</v>
+      </c>
+      <c r="P8" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="17">
         <v>4.5</v>
       </c>
       <c r="R8" s="4">
@@ -2343,7 +2289,7 @@
       <c r="T8" s="4">
         <v>0</v>
       </c>
-      <c r="U8" s="21">
+      <c r="U8" s="15">
         <v>4.5</v>
       </c>
       <c r="V8" s="3">
@@ -2400,55 +2346,55 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="23">
+        <v>83</v>
+      </c>
+      <c r="C9" s="17">
         <v>8</v>
       </c>
-      <c r="D9" s="23">
-        <v>1</v>
-      </c>
-      <c r="E9" s="25">
-        <v>1</v>
-      </c>
-      <c r="F9" s="26">
+      <c r="D9" s="17">
+        <v>1</v>
+      </c>
+      <c r="E9" s="19">
+        <v>1</v>
+      </c>
+      <c r="F9" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G9" s="25">
-        <v>0</v>
-      </c>
-      <c r="H9" s="23">
-        <v>0</v>
-      </c>
-      <c r="I9" s="23">
-        <v>0</v>
-      </c>
-      <c r="J9" s="23">
+      <c r="G9" s="19">
+        <v>0</v>
+      </c>
+      <c r="H9" s="17">
+        <v>0</v>
+      </c>
+      <c r="I9" s="17">
+        <v>0</v>
+      </c>
+      <c r="J9" s="17">
         <v>4</v>
       </c>
-      <c r="K9" s="27">
+      <c r="K9" s="21">
         <v>0.4</v>
       </c>
-      <c r="L9" s="27">
+      <c r="L9" s="21">
         <v>0.75</v>
       </c>
-      <c r="M9" s="23">
-        <v>0</v>
-      </c>
-      <c r="N9" s="23">
-        <v>0</v>
-      </c>
-      <c r="O9" s="23">
-        <v>0</v>
-      </c>
-      <c r="P9" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="23">
+      <c r="M9" s="17">
+        <v>0</v>
+      </c>
+      <c r="N9" s="17">
+        <v>0</v>
+      </c>
+      <c r="O9" s="17">
+        <v>0</v>
+      </c>
+      <c r="P9" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="17">
         <v>4.5</v>
       </c>
       <c r="R9" s="4">
@@ -2460,7 +2406,7 @@
       <c r="T9" s="4">
         <v>0</v>
       </c>
-      <c r="U9" s="21">
+      <c r="U9" s="15">
         <v>4.5</v>
       </c>
       <c r="V9" s="3">
@@ -2517,55 +2463,55 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" s="23">
+        <v>84</v>
+      </c>
+      <c r="C10" s="17">
         <v>9</v>
       </c>
-      <c r="D10" s="23">
-        <v>1</v>
-      </c>
-      <c r="E10" s="25">
-        <v>1</v>
-      </c>
-      <c r="F10" s="26">
+      <c r="D10" s="17">
+        <v>1</v>
+      </c>
+      <c r="E10" s="19">
+        <v>1</v>
+      </c>
+      <c r="F10" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G10" s="25">
-        <v>0</v>
-      </c>
-      <c r="H10" s="23">
-        <v>0</v>
-      </c>
-      <c r="I10" s="23">
-        <v>0</v>
-      </c>
-      <c r="J10" s="23">
-        <v>1</v>
-      </c>
-      <c r="K10" s="27">
+      <c r="G10" s="19">
+        <v>0</v>
+      </c>
+      <c r="H10" s="17">
+        <v>0</v>
+      </c>
+      <c r="I10" s="17">
+        <v>0</v>
+      </c>
+      <c r="J10" s="17">
+        <v>1</v>
+      </c>
+      <c r="K10" s="21">
         <v>0.4</v>
       </c>
-      <c r="L10" s="27">
+      <c r="L10" s="21">
         <v>0.75</v>
       </c>
-      <c r="M10" s="23">
-        <v>0</v>
-      </c>
-      <c r="N10" s="23">
-        <v>0</v>
-      </c>
-      <c r="O10" s="23">
-        <v>0</v>
-      </c>
-      <c r="P10" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="23">
+      <c r="M10" s="17">
+        <v>0</v>
+      </c>
+      <c r="N10" s="17">
+        <v>0</v>
+      </c>
+      <c r="O10" s="17">
+        <v>0</v>
+      </c>
+      <c r="P10" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="17">
         <v>4.5</v>
       </c>
       <c r="R10" s="4">
@@ -2577,7 +2523,7 @@
       <c r="T10" s="4">
         <v>0</v>
       </c>
-      <c r="U10" s="21">
+      <c r="U10" s="15">
         <v>4.5</v>
       </c>
       <c r="V10" s="3">
@@ -2637,52 +2583,52 @@
         <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" s="23">
+        <v>106</v>
+      </c>
+      <c r="C11" s="17">
         <v>10</v>
       </c>
-      <c r="D11" s="23">
-        <v>1</v>
-      </c>
-      <c r="E11" s="25">
-        <v>1</v>
-      </c>
-      <c r="F11" s="26">
+      <c r="D11" s="17">
+        <v>1</v>
+      </c>
+      <c r="E11" s="19">
+        <v>1</v>
+      </c>
+      <c r="F11" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G11" s="25">
-        <v>0</v>
-      </c>
-      <c r="H11" s="23">
-        <v>0</v>
-      </c>
-      <c r="I11" s="23">
-        <v>0</v>
-      </c>
-      <c r="J11" s="23">
-        <v>0</v>
-      </c>
-      <c r="K11" s="23">
-        <v>0</v>
-      </c>
-      <c r="L11" s="23">
-        <v>0</v>
-      </c>
-      <c r="M11" s="23">
-        <v>0</v>
-      </c>
-      <c r="N11" s="23">
-        <v>1</v>
-      </c>
-      <c r="O11" s="23">
-        <v>0</v>
-      </c>
-      <c r="P11" s="28">
+      <c r="G11" s="19">
+        <v>0</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0</v>
+      </c>
+      <c r="I11" s="17">
+        <v>0</v>
+      </c>
+      <c r="J11" s="17">
+        <v>0</v>
+      </c>
+      <c r="K11" s="17">
+        <v>0</v>
+      </c>
+      <c r="L11" s="17">
+        <v>0</v>
+      </c>
+      <c r="M11" s="17">
+        <v>0</v>
+      </c>
+      <c r="N11" s="17">
+        <v>1</v>
+      </c>
+      <c r="O11" s="17">
+        <v>0</v>
+      </c>
+      <c r="P11" s="22">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="Q11" s="23">
+      <c r="Q11" s="17">
         <v>4.5</v>
       </c>
       <c r="R11" s="4">
@@ -2721,7 +2667,7 @@
       <c r="AC11" s="4">
         <v>0</v>
       </c>
-      <c r="AD11" s="21">
+      <c r="AD11" s="15">
         <v>4.5</v>
       </c>
       <c r="AE11" s="3">
@@ -2754,52 +2700,52 @@
         <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="23">
+        <v>107</v>
+      </c>
+      <c r="C12" s="17">
         <v>11</v>
       </c>
-      <c r="D12" s="23">
-        <v>1</v>
-      </c>
-      <c r="E12" s="25">
-        <v>1</v>
-      </c>
-      <c r="F12" s="26">
+      <c r="D12" s="17">
+        <v>1</v>
+      </c>
+      <c r="E12" s="19">
+        <v>1</v>
+      </c>
+      <c r="F12" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G12" s="25">
-        <v>0</v>
-      </c>
-      <c r="H12" s="23">
-        <v>0</v>
-      </c>
-      <c r="I12" s="23">
-        <v>0</v>
-      </c>
-      <c r="J12" s="23">
-        <v>0</v>
-      </c>
-      <c r="K12" s="23">
-        <v>0</v>
-      </c>
-      <c r="L12" s="23">
-        <v>0</v>
-      </c>
-      <c r="M12" s="23">
-        <v>1</v>
-      </c>
-      <c r="N12" s="23">
-        <v>0</v>
-      </c>
-      <c r="O12" s="23">
-        <v>0</v>
-      </c>
-      <c r="P12" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="23">
+      <c r="G12" s="19">
+        <v>0</v>
+      </c>
+      <c r="H12" s="17">
+        <v>0</v>
+      </c>
+      <c r="I12" s="17">
+        <v>0</v>
+      </c>
+      <c r="J12" s="17">
+        <v>0</v>
+      </c>
+      <c r="K12" s="17">
+        <v>0</v>
+      </c>
+      <c r="L12" s="17">
+        <v>0</v>
+      </c>
+      <c r="M12" s="17">
+        <v>1</v>
+      </c>
+      <c r="N12" s="17">
+        <v>0</v>
+      </c>
+      <c r="O12" s="17">
+        <v>0</v>
+      </c>
+      <c r="P12" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="17">
         <v>5</v>
       </c>
       <c r="R12" s="4">
@@ -2838,7 +2784,7 @@
       <c r="AC12" s="4">
         <v>0</v>
       </c>
-      <c r="AD12" s="21">
+      <c r="AD12" s="15">
         <v>5</v>
       </c>
       <c r="AE12" s="3">
@@ -2868,55 +2814,55 @@
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="23">
+        <v>85</v>
+      </c>
+      <c r="C13" s="17">
         <v>12</v>
       </c>
-      <c r="D13" s="23">
-        <v>1</v>
-      </c>
-      <c r="E13" s="25">
-        <v>1</v>
-      </c>
-      <c r="F13" s="26">
+      <c r="D13" s="17">
+        <v>1</v>
+      </c>
+      <c r="E13" s="19">
+        <v>1</v>
+      </c>
+      <c r="F13" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G13" s="25">
-        <v>0</v>
-      </c>
-      <c r="H13" s="23">
-        <v>0</v>
-      </c>
-      <c r="I13" s="23">
-        <v>0</v>
-      </c>
-      <c r="J13" s="23">
+      <c r="G13" s="19">
+        <v>0</v>
+      </c>
+      <c r="H13" s="17">
+        <v>0</v>
+      </c>
+      <c r="I13" s="17">
+        <v>0</v>
+      </c>
+      <c r="J13" s="17">
         <v>7</v>
       </c>
-      <c r="K13" s="27">
+      <c r="K13" s="21">
         <v>0.8</v>
       </c>
-      <c r="L13" s="27">
+      <c r="L13" s="21">
         <v>1.35</v>
       </c>
-      <c r="M13" s="23">
-        <v>0</v>
-      </c>
-      <c r="N13" s="23">
-        <v>0</v>
-      </c>
-      <c r="O13" s="23">
-        <v>0</v>
-      </c>
-      <c r="P13" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="23">
+      <c r="M13" s="17">
+        <v>0</v>
+      </c>
+      <c r="N13" s="17">
+        <v>0</v>
+      </c>
+      <c r="O13" s="17">
+        <v>0</v>
+      </c>
+      <c r="P13" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="17">
         <v>5</v>
       </c>
       <c r="R13" s="4">
@@ -2928,7 +2874,7 @@
       <c r="T13" s="4">
         <v>0</v>
       </c>
-      <c r="U13" s="21">
+      <c r="U13" s="15">
         <v>5</v>
       </c>
       <c r="V13" s="3">
@@ -2985,55 +2931,55 @@
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="23">
+        <v>86</v>
+      </c>
+      <c r="C14" s="17">
         <v>13</v>
       </c>
-      <c r="D14" s="23">
-        <v>1</v>
-      </c>
-      <c r="E14" s="25">
-        <v>1</v>
-      </c>
-      <c r="F14" s="26">
+      <c r="D14" s="17">
+        <v>1</v>
+      </c>
+      <c r="E14" s="19">
+        <v>1</v>
+      </c>
+      <c r="F14" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G14" s="25">
-        <v>0</v>
-      </c>
-      <c r="H14" s="23">
-        <v>0</v>
-      </c>
-      <c r="I14" s="23">
-        <v>0</v>
-      </c>
-      <c r="J14" s="23">
+      <c r="G14" s="19">
+        <v>0</v>
+      </c>
+      <c r="H14" s="17">
+        <v>0</v>
+      </c>
+      <c r="I14" s="17">
+        <v>0</v>
+      </c>
+      <c r="J14" s="17">
         <v>7</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="17">
         <v>0.85</v>
       </c>
-      <c r="L14" s="27">
+      <c r="L14" s="21">
         <v>1.35</v>
       </c>
-      <c r="M14" s="23">
-        <v>0</v>
-      </c>
-      <c r="N14" s="23">
-        <v>0</v>
-      </c>
-      <c r="O14" s="23">
-        <v>0</v>
-      </c>
-      <c r="P14" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="23">
+      <c r="M14" s="17">
+        <v>0</v>
+      </c>
+      <c r="N14" s="17">
+        <v>0</v>
+      </c>
+      <c r="O14" s="17">
+        <v>0</v>
+      </c>
+      <c r="P14" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="17">
         <v>5</v>
       </c>
       <c r="R14" s="4">
@@ -3045,7 +2991,7 @@
       <c r="T14" s="4">
         <v>0</v>
       </c>
-      <c r="U14" s="21">
+      <c r="U14" s="15">
         <v>5</v>
       </c>
       <c r="V14" s="3">
@@ -3102,55 +3048,55 @@
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="23">
+        <v>87</v>
+      </c>
+      <c r="C15" s="17">
         <v>14</v>
       </c>
-      <c r="D15" s="23">
-        <v>1</v>
-      </c>
-      <c r="E15" s="25">
-        <v>1</v>
-      </c>
-      <c r="F15" s="26">
+      <c r="D15" s="17">
+        <v>1</v>
+      </c>
+      <c r="E15" s="19">
+        <v>1</v>
+      </c>
+      <c r="F15" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G15" s="25">
-        <v>0</v>
-      </c>
-      <c r="H15" s="23">
-        <v>0</v>
-      </c>
-      <c r="I15" s="23">
-        <v>0</v>
-      </c>
-      <c r="J15" s="23">
+      <c r="G15" s="19">
+        <v>0</v>
+      </c>
+      <c r="H15" s="17">
+        <v>0</v>
+      </c>
+      <c r="I15" s="17">
+        <v>0</v>
+      </c>
+      <c r="J15" s="17">
         <v>4</v>
       </c>
-      <c r="K15" s="27">
+      <c r="K15" s="21">
         <v>0.8</v>
       </c>
-      <c r="L15" s="27">
+      <c r="L15" s="21">
         <v>1.35</v>
       </c>
-      <c r="M15" s="23">
-        <v>0</v>
-      </c>
-      <c r="N15" s="23">
-        <v>0</v>
-      </c>
-      <c r="O15" s="23">
-        <v>0</v>
-      </c>
-      <c r="P15" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="23">
+      <c r="M15" s="17">
+        <v>0</v>
+      </c>
+      <c r="N15" s="17">
+        <v>0</v>
+      </c>
+      <c r="O15" s="17">
+        <v>0</v>
+      </c>
+      <c r="P15" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="17">
         <v>5</v>
       </c>
       <c r="R15" s="4">
@@ -3162,7 +3108,7 @@
       <c r="T15" s="4">
         <v>0</v>
       </c>
-      <c r="U15" s="21">
+      <c r="U15" s="15">
         <v>5</v>
       </c>
       <c r="V15" s="3">
@@ -3219,55 +3165,55 @@
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16" s="23">
+        <v>88</v>
+      </c>
+      <c r="C16" s="17">
         <v>15</v>
       </c>
-      <c r="D16" s="23">
-        <v>1</v>
-      </c>
-      <c r="E16" s="25">
-        <v>1</v>
-      </c>
-      <c r="F16" s="26">
+      <c r="D16" s="17">
+        <v>1</v>
+      </c>
+      <c r="E16" s="19">
+        <v>1</v>
+      </c>
+      <c r="F16" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G16" s="25">
-        <v>0</v>
-      </c>
-      <c r="H16" s="23">
-        <v>0</v>
-      </c>
-      <c r="I16" s="23">
-        <v>0</v>
-      </c>
-      <c r="J16" s="23">
-        <v>1</v>
-      </c>
-      <c r="K16" s="27">
+      <c r="G16" s="19">
+        <v>0</v>
+      </c>
+      <c r="H16" s="17">
+        <v>0</v>
+      </c>
+      <c r="I16" s="17">
+        <v>0</v>
+      </c>
+      <c r="J16" s="17">
+        <v>1</v>
+      </c>
+      <c r="K16" s="21">
         <v>0.8</v>
       </c>
-      <c r="L16" s="27">
+      <c r="L16" s="21">
         <v>1.35</v>
       </c>
-      <c r="M16" s="23">
-        <v>0</v>
-      </c>
-      <c r="N16" s="23">
-        <v>0</v>
-      </c>
-      <c r="O16" s="23">
-        <v>0</v>
-      </c>
-      <c r="P16" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="23">
+      <c r="M16" s="17">
+        <v>0</v>
+      </c>
+      <c r="N16" s="17">
+        <v>0</v>
+      </c>
+      <c r="O16" s="17">
+        <v>0</v>
+      </c>
+      <c r="P16" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="17">
         <v>5</v>
       </c>
       <c r="R16" s="4">
@@ -3279,7 +3225,7 @@
       <c r="T16" s="4">
         <v>0</v>
       </c>
-      <c r="U16" s="21">
+      <c r="U16" s="15">
         <v>5</v>
       </c>
       <c r="V16" s="3">
@@ -3339,52 +3285,52 @@
         <v>37</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="23">
+        <v>104</v>
+      </c>
+      <c r="C17" s="17">
         <v>16</v>
       </c>
-      <c r="D17" s="23">
-        <v>1</v>
-      </c>
-      <c r="E17" s="25">
-        <v>1</v>
-      </c>
-      <c r="F17" s="26">
+      <c r="D17" s="17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="19">
+        <v>1</v>
+      </c>
+      <c r="F17" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G17" s="25">
-        <v>0</v>
-      </c>
-      <c r="H17" s="23">
-        <v>0</v>
-      </c>
-      <c r="I17" s="23">
-        <v>0</v>
-      </c>
-      <c r="J17" s="23">
-        <v>0</v>
-      </c>
-      <c r="K17" s="23">
-        <v>0</v>
-      </c>
-      <c r="L17" s="23">
-        <v>0</v>
-      </c>
-      <c r="M17" s="23">
-        <v>0</v>
-      </c>
-      <c r="N17" s="23">
-        <v>1</v>
-      </c>
-      <c r="O17" s="23">
-        <v>0</v>
-      </c>
-      <c r="P17" s="28">
+      <c r="G17" s="19">
+        <v>0</v>
+      </c>
+      <c r="H17" s="17">
+        <v>0</v>
+      </c>
+      <c r="I17" s="17">
+        <v>0</v>
+      </c>
+      <c r="J17" s="17">
+        <v>0</v>
+      </c>
+      <c r="K17" s="17">
+        <v>0</v>
+      </c>
+      <c r="L17" s="17">
+        <v>0</v>
+      </c>
+      <c r="M17" s="17">
+        <v>0</v>
+      </c>
+      <c r="N17" s="17">
+        <v>1</v>
+      </c>
+      <c r="O17" s="17">
+        <v>0</v>
+      </c>
+      <c r="P17" s="22">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="Q17" s="23">
+      <c r="Q17" s="17">
         <v>6.5</v>
       </c>
       <c r="R17" s="4">
@@ -3409,12 +3355,12 @@
         <v>4.5</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z17" s="1">
         <v>0</v>
       </c>
-      <c r="AA17" s="21">
+      <c r="AA17" s="15">
         <v>6.5</v>
       </c>
       <c r="AB17" s="6" t="s">
@@ -3456,52 +3402,52 @@
         <v>36</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C18" s="23">
+        <v>105</v>
+      </c>
+      <c r="C18" s="17">
         <v>17</v>
       </c>
-      <c r="D18" s="23">
-        <v>1</v>
-      </c>
-      <c r="E18" s="25">
+      <c r="D18" s="17">
+        <v>1</v>
+      </c>
+      <c r="E18" s="19">
         <v>0.7</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G18" s="25">
-        <v>0</v>
-      </c>
-      <c r="H18" s="23">
-        <v>0</v>
-      </c>
-      <c r="I18" s="23">
-        <v>0</v>
-      </c>
-      <c r="J18" s="23">
-        <v>0</v>
-      </c>
-      <c r="K18" s="23">
-        <v>0</v>
-      </c>
-      <c r="L18" s="23">
-        <v>0</v>
-      </c>
-      <c r="M18" s="23">
-        <v>0</v>
-      </c>
-      <c r="N18" s="23">
-        <v>0</v>
-      </c>
-      <c r="O18" s="23">
-        <v>1</v>
-      </c>
-      <c r="P18" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="23">
+      <c r="G18" s="19">
+        <v>0</v>
+      </c>
+      <c r="H18" s="17">
+        <v>0</v>
+      </c>
+      <c r="I18" s="17">
+        <v>0</v>
+      </c>
+      <c r="J18" s="17">
+        <v>0</v>
+      </c>
+      <c r="K18" s="17">
+        <v>0</v>
+      </c>
+      <c r="L18" s="17">
+        <v>0</v>
+      </c>
+      <c r="M18" s="17">
+        <v>0</v>
+      </c>
+      <c r="N18" s="17">
+        <v>0</v>
+      </c>
+      <c r="O18" s="17">
+        <v>1</v>
+      </c>
+      <c r="P18" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="17">
         <v>10</v>
       </c>
       <c r="R18" s="4">
@@ -3549,7 +3495,7 @@
       <c r="AF18" s="4">
         <v>0</v>
       </c>
-      <c r="AG18" s="21">
+      <c r="AG18" s="15">
         <v>10</v>
       </c>
       <c r="AH18" s="3">
@@ -3570,25 +3516,25 @@
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="23">
+        <v>98</v>
+      </c>
+      <c r="C19" s="17">
         <v>18</v>
       </c>
-      <c r="D19" s="23">
-        <v>1</v>
-      </c>
-      <c r="E19" s="25">
+      <c r="D19" s="17">
+        <v>1</v>
+      </c>
+      <c r="E19" s="19">
         <v>0.7</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="19">
         <v>0</v>
       </c>
       <c r="H19" s="7">
@@ -3657,7 +3603,7 @@
       <c r="AC19" s="4">
         <v>0</v>
       </c>
-      <c r="AD19" s="21">
+      <c r="AD19" s="15">
         <v>18</v>
       </c>
       <c r="AE19" s="3">
@@ -3687,25 +3633,25 @@
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="23">
+        <v>99</v>
+      </c>
+      <c r="C20" s="17">
         <v>19</v>
       </c>
-      <c r="D20" s="23">
-        <v>1</v>
-      </c>
-      <c r="E20" s="25">
+      <c r="D20" s="17">
+        <v>1</v>
+      </c>
+      <c r="E20" s="19">
         <v>0.7</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="19">
         <v>0</v>
       </c>
       <c r="H20" s="7">
@@ -3742,7 +3688,7 @@
         <v>3</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T20" s="2" t="s">
         <v>27</v>
@@ -3751,7 +3697,7 @@
         <v>6</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W20" s="1">
         <v>0</v>
@@ -3769,12 +3715,12 @@
         <v>14.5</v>
       </c>
       <c r="AB20" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AC20" s="4">
         <v>0</v>
       </c>
-      <c r="AD20" s="21">
+      <c r="AD20" s="15">
         <v>18</v>
       </c>
       <c r="AE20" s="3">
@@ -3804,55 +3750,55 @@
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="23">
+        <v>102</v>
+      </c>
+      <c r="C21" s="17">
         <v>20</v>
       </c>
-      <c r="D21" s="23">
-        <v>1</v>
-      </c>
-      <c r="E21" s="25">
-        <v>1</v>
-      </c>
-      <c r="F21" s="26">
+      <c r="D21" s="17">
+        <v>1</v>
+      </c>
+      <c r="E21" s="19">
+        <v>1</v>
+      </c>
+      <c r="F21" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="19">
         <v>-0.33</v>
       </c>
-      <c r="H21" s="23">
-        <v>0</v>
-      </c>
-      <c r="I21" s="23">
-        <v>0</v>
-      </c>
-      <c r="J21" s="23">
-        <v>0</v>
-      </c>
-      <c r="K21" s="23">
-        <v>0</v>
-      </c>
-      <c r="L21" s="23">
-        <v>0</v>
-      </c>
-      <c r="M21" s="23">
-        <v>0</v>
-      </c>
-      <c r="N21" s="23">
-        <v>1</v>
-      </c>
-      <c r="O21" s="23">
-        <v>0</v>
-      </c>
-      <c r="P21" s="28">
+      <c r="H21" s="17">
+        <v>0</v>
+      </c>
+      <c r="I21" s="17">
+        <v>0</v>
+      </c>
+      <c r="J21" s="17">
+        <v>0</v>
+      </c>
+      <c r="K21" s="17">
+        <v>0</v>
+      </c>
+      <c r="L21" s="17">
+        <v>0</v>
+      </c>
+      <c r="M21" s="17">
+        <v>0</v>
+      </c>
+      <c r="N21" s="17">
+        <v>1</v>
+      </c>
+      <c r="O21" s="17">
+        <v>0</v>
+      </c>
+      <c r="P21" s="22">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="Q21" s="23">
+      <c r="Q21" s="17">
         <v>30</v>
       </c>
       <c r="R21" s="4">
@@ -3877,7 +3823,7 @@
         <v>17</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Z21" s="1">
         <v>0</v>
@@ -3891,7 +3837,7 @@
       <c r="AC21" s="4">
         <v>0</v>
       </c>
-      <c r="AD21" s="21">
+      <c r="AD21" s="15">
         <v>30</v>
       </c>
       <c r="AE21" s="3">
@@ -3921,55 +3867,55 @@
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C22" s="23">
+        <v>103</v>
+      </c>
+      <c r="C22" s="17">
         <v>21</v>
       </c>
-      <c r="D22" s="23">
-        <v>1</v>
-      </c>
-      <c r="E22" s="25">
-        <v>1</v>
-      </c>
-      <c r="F22" s="26">
+      <c r="D22" s="17">
+        <v>1</v>
+      </c>
+      <c r="E22" s="19">
+        <v>1</v>
+      </c>
+      <c r="F22" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="19">
         <v>0.33</v>
       </c>
-      <c r="H22" s="23">
-        <v>0</v>
-      </c>
-      <c r="I22" s="23">
-        <v>0</v>
-      </c>
-      <c r="J22" s="23">
-        <v>0</v>
-      </c>
-      <c r="K22" s="23">
-        <v>0</v>
-      </c>
-      <c r="L22" s="23">
-        <v>0</v>
-      </c>
-      <c r="M22" s="23">
-        <v>0</v>
-      </c>
-      <c r="N22" s="23">
-        <v>1</v>
-      </c>
-      <c r="O22" s="23">
-        <v>0</v>
-      </c>
-      <c r="P22" s="28">
+      <c r="H22" s="17">
+        <v>0</v>
+      </c>
+      <c r="I22" s="17">
+        <v>0</v>
+      </c>
+      <c r="J22" s="17">
+        <v>0</v>
+      </c>
+      <c r="K22" s="17">
+        <v>0</v>
+      </c>
+      <c r="L22" s="17">
+        <v>0</v>
+      </c>
+      <c r="M22" s="17">
+        <v>0</v>
+      </c>
+      <c r="N22" s="17">
+        <v>1</v>
+      </c>
+      <c r="O22" s="17">
+        <v>0</v>
+      </c>
+      <c r="P22" s="22">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="Q22" s="23">
+      <c r="Q22" s="17">
         <v>30</v>
       </c>
       <c r="R22" s="4">
@@ -4008,7 +3954,7 @@
       <c r="AC22" s="4">
         <v>0</v>
       </c>
-      <c r="AD22" s="21">
+      <c r="AD22" s="15">
         <v>30</v>
       </c>
       <c r="AE22" s="3">
@@ -4041,58 +3987,58 @@
         <v>40</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="23">
+        <v>96</v>
+      </c>
+      <c r="C23" s="17">
         <v>22</v>
       </c>
-      <c r="D23" s="23">
-        <v>1</v>
-      </c>
-      <c r="E23" s="25">
-        <v>1</v>
-      </c>
-      <c r="F23" s="29">
+      <c r="D23" s="17">
+        <v>1</v>
+      </c>
+      <c r="E23" s="19">
+        <v>1</v>
+      </c>
+      <c r="F23" s="23">
         <f>Input!H2</f>
         <v>1</v>
       </c>
-      <c r="G23" s="25">
-        <v>1</v>
-      </c>
-      <c r="H23" s="23">
-        <v>0</v>
-      </c>
-      <c r="I23" s="23">
-        <v>0</v>
-      </c>
-      <c r="J23" s="23">
-        <v>0</v>
-      </c>
-      <c r="K23" s="23">
-        <v>0</v>
-      </c>
-      <c r="L23" s="23">
-        <v>0</v>
-      </c>
-      <c r="M23" s="23">
-        <v>0</v>
-      </c>
-      <c r="N23" s="23">
-        <v>1</v>
-      </c>
-      <c r="O23" s="23">
-        <v>0</v>
-      </c>
-      <c r="P23" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="23">
+      <c r="G23" s="19">
+        <v>1</v>
+      </c>
+      <c r="H23" s="17">
+        <v>0</v>
+      </c>
+      <c r="I23" s="17">
+        <v>0</v>
+      </c>
+      <c r="J23" s="17">
+        <v>0</v>
+      </c>
+      <c r="K23" s="17">
+        <v>0</v>
+      </c>
+      <c r="L23" s="17">
+        <v>0</v>
+      </c>
+      <c r="M23" s="17">
+        <v>0</v>
+      </c>
+      <c r="N23" s="17">
+        <v>1</v>
+      </c>
+      <c r="O23" s="17">
+        <v>0</v>
+      </c>
+      <c r="P23" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="17">
         <v>52</v>
       </c>
       <c r="R23" s="4">
         <v>3</v>
       </c>
-      <c r="S23" s="34">
+      <c r="S23" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) + 0.025</f>
         <v>1.0316739272428239</v>
       </c>
@@ -4102,7 +4048,7 @@
       <c r="U23" s="1">
         <v>10</v>
       </c>
-      <c r="V23" s="34">
+      <c r="V23" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) - 0.025</f>
         <v>0.98167392724282398</v>
       </c>
@@ -4112,7 +4058,7 @@
       <c r="X23" s="1">
         <v>17</v>
       </c>
-      <c r="Y23" s="34">
+      <c r="Y23" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2)</f>
         <v>1.006673927242824</v>
       </c>
@@ -4122,7 +4068,7 @@
       <c r="AA23" s="1">
         <v>24</v>
       </c>
-      <c r="AB23" s="34">
+      <c r="AB23" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) + 0.05</f>
         <v>1.0566739272428241</v>
       </c>
@@ -4132,7 +4078,7 @@
       <c r="AD23" s="4">
         <v>31</v>
       </c>
-      <c r="AE23" s="34">
+      <c r="AE23" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2)</f>
         <v>1.006673927242824</v>
       </c>
@@ -4142,7 +4088,7 @@
       <c r="AG23" s="1">
         <v>38</v>
       </c>
-      <c r="AH23" s="34">
+      <c r="AH23" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) - 0.05</f>
         <v>0.95667392724282396</v>
       </c>
@@ -4152,7 +4098,7 @@
       <c r="AJ23" s="1">
         <v>45</v>
       </c>
-      <c r="AK23" s="34">
+      <c r="AK23" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2)</f>
         <v>1.006673927242824</v>
       </c>
@@ -4162,25 +4108,25 @@
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="23">
+        <v>93</v>
+      </c>
+      <c r="C24" s="17">
         <v>23</v>
       </c>
-      <c r="D24" s="23">
-        <v>1</v>
-      </c>
-      <c r="E24" s="25">
+      <c r="D24" s="17">
+        <v>1</v>
+      </c>
+      <c r="E24" s="19">
         <v>0.7</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="19">
         <v>0</v>
       </c>
       <c r="H24" s="7">
@@ -4210,7 +4156,7 @@
       <c r="P24" s="7">
         <v>1</v>
       </c>
-      <c r="Q24" s="12">
+      <c r="Q24" s="8">
         <v>80</v>
       </c>
       <c r="R24" s="4">
@@ -4222,7 +4168,7 @@
       <c r="T24" s="1">
         <v>0</v>
       </c>
-      <c r="U24" s="20">
+      <c r="U24" s="14">
         <v>80</v>
       </c>
       <c r="V24" s="3">
@@ -4279,25 +4225,25 @@
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="23">
+        <v>90</v>
+      </c>
+      <c r="C25" s="17">
         <v>24</v>
       </c>
-      <c r="D25" s="23">
-        <v>1</v>
-      </c>
-      <c r="E25" s="25">
+      <c r="D25" s="17">
+        <v>1</v>
+      </c>
+      <c r="E25" s="19">
         <v>0.5</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F25" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="19">
         <v>0</v>
       </c>
       <c r="H25" s="7">
@@ -4327,7 +4273,7 @@
       <c r="P25" s="7">
         <v>1</v>
       </c>
-      <c r="Q25" s="12">
+      <c r="Q25" s="8">
         <v>80</v>
       </c>
       <c r="R25" s="4">
@@ -4339,7 +4285,7 @@
       <c r="T25" s="1">
         <v>0</v>
       </c>
-      <c r="U25" s="20">
+      <c r="U25" s="14">
         <v>80</v>
       </c>
       <c r="V25" s="3">
@@ -4393,7 +4339,7 @@
       <c r="AL25" s="3">
         <v>0</v>
       </c>
-      <c r="AQ25" s="34">
+      <c r="AQ25" s="28">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) + 0.025</f>
         <v>1.0316739272428239</v>
       </c>
@@ -4403,52 +4349,52 @@
         <v>35</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="23">
+        <v>100</v>
+      </c>
+      <c r="C26" s="17">
         <v>25</v>
       </c>
-      <c r="D26" s="23">
-        <v>1</v>
-      </c>
-      <c r="E26" s="25">
+      <c r="D26" s="17">
+        <v>1</v>
+      </c>
+      <c r="E26" s="19">
         <v>0.7</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G26" s="25">
-        <v>0</v>
-      </c>
-      <c r="H26" s="23">
-        <v>0</v>
-      </c>
-      <c r="I26" s="23">
-        <v>0</v>
-      </c>
-      <c r="J26" s="23">
-        <v>0</v>
-      </c>
-      <c r="K26" s="23">
-        <v>0</v>
-      </c>
-      <c r="L26" s="23">
-        <v>0</v>
-      </c>
-      <c r="M26" s="23">
-        <v>0</v>
-      </c>
-      <c r="N26" s="23">
-        <v>0</v>
-      </c>
-      <c r="O26" s="23">
-        <v>1</v>
-      </c>
-      <c r="P26" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="23">
+      <c r="G26" s="19">
+        <v>0</v>
+      </c>
+      <c r="H26" s="17">
+        <v>0</v>
+      </c>
+      <c r="I26" s="17">
+        <v>0</v>
+      </c>
+      <c r="J26" s="17">
+        <v>0</v>
+      </c>
+      <c r="K26" s="17">
+        <v>0</v>
+      </c>
+      <c r="L26" s="17">
+        <v>0</v>
+      </c>
+      <c r="M26" s="17">
+        <v>0</v>
+      </c>
+      <c r="N26" s="17">
+        <v>0</v>
+      </c>
+      <c r="O26" s="17">
+        <v>1</v>
+      </c>
+      <c r="P26" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="17">
         <v>80</v>
       </c>
       <c r="R26" s="4">
@@ -4473,7 +4419,7 @@
         <v>42</v>
       </c>
       <c r="Y26" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z26" s="1">
         <v>0</v>
@@ -4487,7 +4433,7 @@
       <c r="AC26" s="4">
         <v>0</v>
       </c>
-      <c r="AD26" s="21">
+      <c r="AD26" s="15">
         <v>80</v>
       </c>
       <c r="AE26" s="3">
@@ -4520,52 +4466,52 @@
         <v>39</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="23">
+        <v>101</v>
+      </c>
+      <c r="C27" s="17">
         <v>26</v>
       </c>
-      <c r="D27" s="23">
-        <v>1</v>
-      </c>
-      <c r="E27" s="25">
+      <c r="D27" s="17">
+        <v>1</v>
+      </c>
+      <c r="E27" s="19">
         <v>0.7</v>
       </c>
-      <c r="F27" s="26">
+      <c r="F27" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G27" s="25">
-        <v>0</v>
-      </c>
-      <c r="H27" s="23">
-        <v>0</v>
-      </c>
-      <c r="I27" s="23">
-        <v>0</v>
-      </c>
-      <c r="J27" s="23">
-        <v>0</v>
-      </c>
-      <c r="K27" s="23">
-        <v>0</v>
-      </c>
-      <c r="L27" s="23">
-        <v>0</v>
-      </c>
-      <c r="M27" s="23">
-        <v>0</v>
-      </c>
-      <c r="N27" s="23">
-        <v>0</v>
-      </c>
-      <c r="O27" s="23">
-        <v>1</v>
-      </c>
-      <c r="P27" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="23">
+      <c r="G27" s="19">
+        <v>0</v>
+      </c>
+      <c r="H27" s="17">
+        <v>0</v>
+      </c>
+      <c r="I27" s="17">
+        <v>0</v>
+      </c>
+      <c r="J27" s="17">
+        <v>0</v>
+      </c>
+      <c r="K27" s="17">
+        <v>0</v>
+      </c>
+      <c r="L27" s="17">
+        <v>0</v>
+      </c>
+      <c r="M27" s="17">
+        <v>0</v>
+      </c>
+      <c r="N27" s="17">
+        <v>0</v>
+      </c>
+      <c r="O27" s="17">
+        <v>1</v>
+      </c>
+      <c r="P27" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="17">
         <v>80</v>
       </c>
       <c r="R27" s="4">
@@ -4590,7 +4536,7 @@
         <v>42</v>
       </c>
       <c r="Y27" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z27" s="1">
         <v>0</v>
@@ -4604,7 +4550,7 @@
       <c r="AC27" s="4">
         <v>0</v>
       </c>
-      <c r="AD27" s="21">
+      <c r="AD27" s="15">
         <v>80</v>
       </c>
       <c r="AE27" s="3">
@@ -4634,25 +4580,25 @@
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C28" s="23">
+        <v>92</v>
+      </c>
+      <c r="C28" s="17">
         <v>27</v>
       </c>
-      <c r="D28" s="23">
-        <v>1</v>
-      </c>
-      <c r="E28" s="25">
-        <v>1</v>
-      </c>
-      <c r="F28" s="26">
+      <c r="D28" s="17">
+        <v>1</v>
+      </c>
+      <c r="E28" s="19">
+        <v>1</v>
+      </c>
+      <c r="F28" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="19">
         <v>0</v>
       </c>
       <c r="H28" s="7">
@@ -4682,7 +4628,7 @@
       <c r="P28" s="7">
         <v>1</v>
       </c>
-      <c r="Q28" s="12">
+      <c r="Q28" s="8">
         <v>100</v>
       </c>
       <c r="R28" s="4">
@@ -4694,7 +4640,7 @@
       <c r="T28" s="1">
         <v>0</v>
       </c>
-      <c r="U28" s="20">
+      <c r="U28" s="14">
         <v>100</v>
       </c>
       <c r="V28" s="3">
@@ -4751,25 +4697,25 @@
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="23">
+        <v>91</v>
+      </c>
+      <c r="C29" s="17">
         <v>28</v>
       </c>
-      <c r="D29" s="23">
-        <v>1</v>
-      </c>
-      <c r="E29" s="25">
+      <c r="D29" s="17">
+        <v>1</v>
+      </c>
+      <c r="E29" s="19">
         <v>0.7</v>
       </c>
-      <c r="F29" s="26">
+      <c r="F29" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G29" s="25">
+      <c r="G29" s="19">
         <v>0</v>
       </c>
       <c r="H29" s="7">
@@ -4799,7 +4745,7 @@
       <c r="P29" s="7">
         <v>1</v>
       </c>
-      <c r="Q29" s="12">
+      <c r="Q29" s="8">
         <v>100</v>
       </c>
       <c r="R29" s="4">
@@ -4811,7 +4757,7 @@
       <c r="T29" s="1">
         <v>0</v>
       </c>
-      <c r="U29" s="20">
+      <c r="U29" s="14">
         <v>100</v>
       </c>
       <c r="V29" s="3">
@@ -4871,22 +4817,22 @@
         <v>41</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C30" s="23">
+        <v>97</v>
+      </c>
+      <c r="C30" s="17">
         <v>29</v>
       </c>
-      <c r="D30" s="23">
-        <v>1</v>
-      </c>
-      <c r="E30" s="25">
+      <c r="D30" s="17">
+        <v>1</v>
+      </c>
+      <c r="E30" s="19">
         <v>0.3</v>
       </c>
-      <c r="F30" s="29">
+      <c r="F30" s="23">
         <f>Input!I2</f>
         <v>2</v>
       </c>
-      <c r="G30" s="25">
+      <c r="G30" s="19">
         <v>0.99</v>
       </c>
       <c r="H30" s="7">
@@ -4955,7 +4901,7 @@
       <c r="AC30" s="1">
         <v>0</v>
       </c>
-      <c r="AD30" s="21">
+      <c r="AD30" s="15">
         <v>140</v>
       </c>
       <c r="AE30" s="3">
@@ -4988,22 +4934,22 @@
         <v>38</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" s="23">
+        <v>95</v>
+      </c>
+      <c r="C31" s="17">
         <v>30</v>
       </c>
-      <c r="D31" s="23">
-        <v>1</v>
-      </c>
-      <c r="E31" s="25">
-        <v>1</v>
-      </c>
-      <c r="F31" s="26">
+      <c r="D31" s="17">
+        <v>1</v>
+      </c>
+      <c r="E31" s="19">
+        <v>1</v>
+      </c>
+      <c r="F31" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G31" s="25">
+      <c r="G31" s="19">
         <v>0</v>
       </c>
       <c r="H31" s="7">
@@ -5072,7 +5018,7 @@
       <c r="AC31" s="1">
         <v>0</v>
       </c>
-      <c r="AD31" s="21">
+      <c r="AD31" s="15">
         <v>145</v>
       </c>
       <c r="AE31" s="3">
@@ -5105,22 +5051,22 @@
         <v>38</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C32" s="23">
+        <v>94</v>
+      </c>
+      <c r="C32" s="17">
         <v>31</v>
       </c>
-      <c r="D32" s="23">
-        <v>1</v>
-      </c>
-      <c r="E32" s="25">
-        <v>1</v>
-      </c>
-      <c r="F32" s="26">
+      <c r="D32" s="17">
+        <v>1</v>
+      </c>
+      <c r="E32" s="19">
+        <v>1</v>
+      </c>
+      <c r="F32" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G32" s="25">
+      <c r="G32" s="19">
         <v>0</v>
       </c>
       <c r="H32" s="7">
@@ -5189,7 +5135,7 @@
       <c r="AC32" s="1">
         <v>0</v>
       </c>
-      <c r="AD32" s="21">
+      <c r="AD32" s="15">
         <v>145</v>
       </c>
       <c r="AE32" s="3">
@@ -5219,25 +5165,25 @@
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" s="23">
+        <v>89</v>
+      </c>
+      <c r="C33" s="17">
         <v>32</v>
       </c>
-      <c r="D33" s="23">
-        <v>1</v>
-      </c>
-      <c r="E33" s="25">
-        <v>0</v>
-      </c>
-      <c r="F33" s="26">
+      <c r="D33" s="17">
+        <v>1</v>
+      </c>
+      <c r="E33" s="19">
+        <v>0</v>
+      </c>
+      <c r="F33" s="20">
         <f>Input!G2</f>
         <v>0</v>
       </c>
-      <c r="G33" s="25">
+      <c r="G33" s="19">
         <v>0</v>
       </c>
       <c r="H33" s="7">
@@ -5279,7 +5225,7 @@
       <c r="T33" s="1">
         <v>0</v>
       </c>
-      <c r="U33" s="21">
+      <c r="U33" s="15">
         <v>155</v>
       </c>
       <c r="V33" s="3">
@@ -5351,92 +5297,92 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E2 E4 E6 E8 E10 E12 E14 E16">
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3 E5 E7 E9 E11 E13 E15 E17">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5446,215 +5392,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="44.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="9">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9">
-        <v>0</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="16">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="9">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="9">
-        <v>3</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="9">
-        <v>4</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0.7</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
-        <v>5</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
-        <v>6</v>
-      </c>
-      <c r="C7" s="9">
-        <v>1</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="9">
-        <v>7</v>
-      </c>
-      <c r="C8" s="9">
-        <v>1</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="9">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="9">
-        <v>8</v>
-      </c>
-      <c r="C9" s="9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="9">
-        <v>-0.33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
-        <v>9</v>
-      </c>
-      <c r="C10" s="9">
-        <v>0.6</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="9">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="9">
-        <v>10</v>
-      </c>
-      <c r="C11" s="10">
-        <v>0.6</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="9">
-        <v>-0.33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="9">
-        <v>11</v>
-      </c>
-      <c r="C12" s="10">
-        <v>0.3</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="9">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="9">
-        <v>12</v>
-      </c>
-      <c r="C13" s="10">
-        <v>0.3</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="9">
-        <v>-0.33</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C2:C13">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
@@ -5671,120 +5408,120 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D13" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E13" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E14" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D15" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E15" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E16" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E18" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E19" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E20" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Energinet data removed from "PSCAD compilers" tab
</commit_message>
<xml_diff>
--- a/PSCAD/DK1_DSO_D/TestCases.xlsx
+++ b/PSCAD/DK1_DSO_D/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" tabRatio="350"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="133">
   <si>
     <t>PrefCtrl</t>
   </si>
@@ -423,111 +423,6 @@
   </si>
   <si>
     <t>Note:</t>
-  </si>
-  <si>
-    <t>Servers:</t>
-  </si>
-  <si>
-    <t>X0133P01</t>
-  </si>
-  <si>
-    <t>Y0133P03</t>
-  </si>
-  <si>
-    <t>Y0133P01</t>
-  </si>
-  <si>
-    <t>Y0133P02</t>
-  </si>
-  <si>
-    <t>Compliers:</t>
-  </si>
-  <si>
-    <t>The compliers are different on different servers at Energinet.</t>
-  </si>
-  <si>
-    <r>
-      <t>Intel(R) Visual Fortran Compiler XE 15.0.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>5.280</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Intel(R) Visual Fortran Compiler XE 15.0.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>5.280</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (64-bit)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Intel(R) Visual Fortran Compiler XE 15.0.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.148</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Intel(R) Visual Fortran Compiler XE 15.0.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.148</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (64-bit)</t>
-    </r>
   </si>
   <si>
     <t>See 'PSCAD Compliers' sheet for guidance</t>
@@ -552,7 +447,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -584,14 +479,6 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1269,7 +1156,7 @@
         <v>118</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1298,7 +1185,7 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="K2" t="s">
         <v>123</v>
@@ -1318,10 +1205,10 @@
         <v>127</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="N4" s="26" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -1373,7 +1260,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK24" sqref="AK24"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,7 +1307,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>43</v>
@@ -5393,135 +5280,54 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="5" width="48.140625" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>127</v>
-      </c>
-      <c r="D11" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D13" t="s">
-        <v>129</v>
-      </c>
-      <c r="E13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>130</v>
-      </c>
-      <c r="E14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>133</v>
-      </c>
-      <c r="D15" t="s">
-        <v>120</v>
-      </c>
-      <c r="E15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>121</v>
-      </c>
-      <c r="E16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>122</v>
-      </c>
-      <c r="E17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>119</v>
-      </c>
-      <c r="E18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>135</v>
-      </c>
-      <c r="E19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>136</v>
-      </c>
-      <c r="E20" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>